<commit_message>
Fixed dates. Dates had removed american holidays, not american.
</commit_message>
<xml_diff>
--- a/Stock_data/ticker_date.xlsx
+++ b/Stock_data/ticker_date.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Odin Mjølsnes\Documents\myrepo2\Stock_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5EF23CF-C069-4124-A424-F3D56402B7F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CB23C9-F1B4-49EC-A216-053738B96F2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{350AA195-DF91-4F4A-A14B-BEDADCFFE301}"/>
   </bookViews>
@@ -1981,8 +1981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA26B976-9A87-448C-B3C3-776059C9EE67}">
   <dimension ref="A1:E265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2653,7 +2653,7 @@
         <v>BSPME NO Equity</v>
       </c>
       <c r="D44" s="3">
-        <v>43798</v>
+        <v>43797</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -2668,7 +2668,7 @@
         <v>BON NO Equity</v>
       </c>
       <c r="D45" s="3">
-        <v>43801</v>
+        <v>43798</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
@@ -2683,7 +2683,7 @@
         <v>BOR NO Equity</v>
       </c>
       <c r="D46" s="3">
-        <v>43802</v>
+        <v>43801</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -2698,7 +2698,7 @@
         <v>BDRILL NO Equity</v>
       </c>
       <c r="D47" s="3">
-        <v>43803</v>
+        <v>43802</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -2713,7 +2713,7 @@
         <v>BRG NO Equity</v>
       </c>
       <c r="D48" s="3">
-        <v>43804</v>
+        <v>43803</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
@@ -2728,7 +2728,7 @@
         <v>BOUVET NO Equity</v>
       </c>
       <c r="D49" s="3">
-        <v>43805</v>
+        <v>43804</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
@@ -2743,7 +2743,7 @@
         <v>BRAME NO Equity</v>
       </c>
       <c r="D50" s="3">
-        <v>43808</v>
+        <v>43805</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
@@ -2758,7 +2758,7 @@
         <v>BWE NO Equity</v>
       </c>
       <c r="D51" s="3">
-        <v>43809</v>
+        <v>43808</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
@@ -2773,7 +2773,7 @@
         <v>BWLPG NO Equity</v>
       </c>
       <c r="D52" s="3">
-        <v>43810</v>
+        <v>43809</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
@@ -2788,7 +2788,7 @@
         <v>BWO NO Equity</v>
       </c>
       <c r="D53" s="3">
-        <v>43811</v>
+        <v>43810</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
@@ -2803,7 +2803,7 @@
         <v>BMA NO Equity</v>
       </c>
       <c r="D54" s="3">
-        <v>43812</v>
+        <v>43811</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
@@ -2818,7 +2818,7 @@
         <v>CARA NO Equity</v>
       </c>
       <c r="D55" s="3">
-        <v>43815</v>
+        <v>43812</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
@@ -2833,7 +2833,7 @@
         <v>CLOUDME NO Equity</v>
       </c>
       <c r="D56" s="3">
-        <v>43816</v>
+        <v>43815</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
@@ -2848,7 +2848,7 @@
         <v>COV NO Equity</v>
       </c>
       <c r="D57" s="3">
-        <v>43817</v>
+        <v>43816</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
@@ -2863,7 +2863,7 @@
         <v>CRAYON NO Equity</v>
       </c>
       <c r="D58" s="3">
-        <v>43818</v>
+        <v>43817</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
@@ -2878,7 +2878,7 @@
         <v>DNB NO Equity</v>
       </c>
       <c r="D59" s="3">
-        <v>43819</v>
+        <v>43818</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
@@ -2893,7 +2893,7 @@
         <v>DNO NO Equity</v>
       </c>
       <c r="D60" s="3">
-        <v>43822</v>
+        <v>43819</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
@@ -2908,7 +2908,7 @@
         <v>DOF NO Equity</v>
       </c>
       <c r="D61" s="3">
-        <v>43823</v>
+        <v>43822</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
@@ -2923,7 +2923,7 @@
         <v>EAM NO Equity</v>
       </c>
       <c r="D62" s="3">
-        <v>43825</v>
+        <v>43826</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -2938,7 +2938,7 @@
         <v>EIOF NO Equity</v>
       </c>
       <c r="D63" s="3">
-        <v>43826</v>
+        <v>43829</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
@@ -2953,7 +2953,7 @@
         <v>EMGS NO Equity</v>
       </c>
       <c r="D64" s="3">
-        <v>43829</v>
+        <v>43832</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
@@ -2968,7 +2968,7 @@
         <v>ELE NO Equity</v>
       </c>
       <c r="D65" s="3">
-        <v>43830</v>
+        <v>43833</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
@@ -2983,7 +2983,7 @@
         <v>ELK NO Equity</v>
       </c>
       <c r="D66" s="3">
-        <v>43832</v>
+        <v>43836</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
@@ -2998,7 +2998,7 @@
         <v>ELOPME NO Equity</v>
       </c>
       <c r="D67" s="3">
-        <v>43833</v>
+        <v>43837</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
@@ -3013,7 +3013,7 @@
         <v>EMAS NO Equity</v>
       </c>
       <c r="D68" s="3">
-        <v>43836</v>
+        <v>43838</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
@@ -3028,7 +3028,7 @@
         <v>ENDUR NO Equity</v>
       </c>
       <c r="D69" s="3">
-        <v>43837</v>
+        <v>43839</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
@@ -3043,7 +3043,7 @@
         <v>ENTRA NO Equity</v>
       </c>
       <c r="D70" s="3">
-        <v>43838</v>
+        <v>43840</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
@@ -3058,7 +3058,7 @@
         <v>EPICME NO Equity</v>
       </c>
       <c r="D71" s="3">
-        <v>43839</v>
+        <v>43843</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
@@ -3073,7 +3073,7 @@
         <v>EQNR NO Equity</v>
       </c>
       <c r="D72" s="3">
-        <v>43840</v>
+        <v>43844</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
@@ -3088,7 +3088,7 @@
         <v>EPR NO Equity</v>
       </c>
       <c r="D73" s="3">
-        <v>43843</v>
+        <v>43845</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
@@ -3103,7 +3103,7 @@
         <v>EXTXME NO Equity</v>
       </c>
       <c r="D74" s="3">
-        <v>43844</v>
+        <v>43846</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
@@ -3118,7 +3118,7 @@
         <v>FJORD NO Equity</v>
       </c>
       <c r="D75" s="3">
-        <v>43845</v>
+        <v>43847</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
@@ -3133,7 +3133,7 @@
         <v>FKRAFT NO Equity</v>
       </c>
       <c r="D76" s="3">
-        <v>43846</v>
+        <v>43850</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
@@ -3148,7 +3148,7 @@
         <v>FLNG NO Equity</v>
       </c>
       <c r="D77" s="3">
-        <v>43847</v>
+        <v>43851</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
@@ -3163,7 +3163,7 @@
         <v>FRO NO Equity</v>
       </c>
       <c r="D78" s="3">
-        <v>43851</v>
+        <v>43852</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
@@ -3178,7 +3178,7 @@
         <v>GIG NO Equity</v>
       </c>
       <c r="D79" s="3">
-        <v>43852</v>
+        <v>43853</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
@@ -3193,7 +3193,7 @@
         <v>RISH NO Equity</v>
       </c>
       <c r="D80" s="3">
-        <v>43853</v>
+        <v>43854</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
@@ -3208,7 +3208,7 @@
         <v>GENTME NO Equity</v>
       </c>
       <c r="D81" s="3">
-        <v>43854</v>
+        <v>43857</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
@@ -3223,7 +3223,7 @@
         <v>GJF NO Equity</v>
       </c>
       <c r="D82" s="3">
-        <v>43857</v>
+        <v>43858</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
@@ -3238,7 +3238,7 @@
         <v>GEOSME NO Equity</v>
       </c>
       <c r="D83" s="3">
-        <v>43858</v>
+        <v>43859</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
@@ -3253,7 +3253,7 @@
         <v>GOGL NO Equity</v>
       </c>
       <c r="D84" s="3">
-        <v>43859</v>
+        <v>43860</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
@@ -3268,7 +3268,7 @@
         <v>GOD NO Equity</v>
       </c>
       <c r="D85" s="3">
-        <v>43860</v>
+        <v>43861</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
@@ -3283,7 +3283,7 @@
         <v>GSF NO Equity</v>
       </c>
       <c r="D86" s="3">
-        <v>43861</v>
+        <v>43864</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
@@ -3298,7 +3298,7 @@
         <v>GRONGME NO Equity</v>
       </c>
       <c r="D87" s="3">
-        <v>43864</v>
+        <v>43865</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
@@ -3313,7 +3313,7 @@
         <v>GYL NO Equity</v>
       </c>
       <c r="D88" s="3">
-        <v>43865</v>
+        <v>43866</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
@@ -3328,7 +3328,7 @@
         <v>HAFNIA NO Equity</v>
       </c>
       <c r="D89" s="3">
-        <v>43866</v>
+        <v>43867</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
@@ -3343,7 +3343,7 @@
         <v>HAVI NO Equity</v>
       </c>
       <c r="D90" s="3">
-        <v>43867</v>
+        <v>43868</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
@@ -3358,7 +3358,7 @@
         <v>HYARD NO Equity</v>
       </c>
       <c r="D91" s="3">
-        <v>43868</v>
+        <v>43871</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
@@ -3373,7 +3373,7 @@
         <v>HELG NO Equity</v>
       </c>
       <c r="D92" s="3">
-        <v>43871</v>
+        <v>43872</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
@@ -3388,7 +3388,7 @@
         <v>HEX NO Equity</v>
       </c>
       <c r="D93" s="3">
-        <v>43872</v>
+        <v>43873</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
@@ -3403,7 +3403,7 @@
         <v>HIDDN NO Equity</v>
       </c>
       <c r="D94" s="3">
-        <v>43873</v>
+        <v>43874</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
@@ -3418,7 +3418,7 @@
         <v>HBC NO Equity</v>
       </c>
       <c r="D95" s="3">
-        <v>43874</v>
+        <v>43875</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
@@ -3433,7 +3433,7 @@
         <v>HUNT NO Equity</v>
       </c>
       <c r="D96" s="3">
-        <v>43875</v>
+        <v>43878</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
@@ -4003,7 +4003,7 @@
         <v>NKR NO Equity</v>
       </c>
       <c r="D134" s="3">
-        <v>43930</v>
+        <v>43935</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
@@ -4018,7 +4018,7 @@
         <v>NEL NO Equity</v>
       </c>
       <c r="D135" s="3">
-        <v>43934</v>
+        <v>43936</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
@@ -4033,7 +4033,7 @@
         <v>NEXT NO Equity</v>
       </c>
       <c r="D136" s="3">
-        <v>43935</v>
+        <v>43937</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
@@ -4048,7 +4048,7 @@
         <v>NISBME NO Equity</v>
       </c>
       <c r="D137" s="3">
-        <v>43936</v>
+        <v>43938</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
@@ -4063,7 +4063,7 @@
         <v>NORBIT NO Equity</v>
       </c>
       <c r="D138" s="3">
-        <v>43937</v>
+        <v>43941</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
@@ -4078,7 +4078,7 @@
         <v>NOM NO Equity</v>
       </c>
       <c r="D139" s="3">
-        <v>43938</v>
+        <v>43942</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
@@ -4093,7 +4093,7 @@
         <v>NANO NO Equity</v>
       </c>
       <c r="D140" s="3">
-        <v>43941</v>
+        <v>43943</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
@@ -4108,7 +4108,7 @@
         <v>NOD NO Equity</v>
       </c>
       <c r="D141" s="3">
-        <v>43942</v>
+        <v>43944</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
@@ -4123,7 +4123,7 @@
         <v>NHY NO Equity</v>
       </c>
       <c r="D142" s="3">
-        <v>43943</v>
+        <v>43945</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
@@ -4138,7 +4138,7 @@
         <v>NSKOG NO Equity</v>
       </c>
       <c r="D143" s="3">
-        <v>43944</v>
+        <v>43948</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
@@ -4153,7 +4153,7 @@
         <v>NORTH NO Equity</v>
       </c>
       <c r="D144" s="3">
-        <v>43945</v>
+        <v>43949</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
@@ -4168,7 +4168,7 @@
         <v>NODL NO Equity</v>
       </c>
       <c r="D145" s="3">
-        <v>43948</v>
+        <v>43950</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
@@ -4183,7 +4183,7 @@
         <v>NOL NO Equity</v>
       </c>
       <c r="D146" s="3">
-        <v>43949</v>
+        <v>43951</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
@@ -4198,7 +4198,7 @@
         <v>NRS NO Equity</v>
       </c>
       <c r="D147" s="3">
-        <v>43950</v>
+        <v>43955</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
@@ -4213,7 +4213,7 @@
         <v>NAS NO Equity</v>
       </c>
       <c r="D148" s="3">
-        <v>43951</v>
+        <v>43956</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
@@ -4228,7 +4228,7 @@
         <v>NOR NO Equity</v>
       </c>
       <c r="D149" s="3">
-        <v>43952</v>
+        <v>43957</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
@@ -4243,7 +4243,7 @@
         <v>NOFI NO Equity</v>
       </c>
       <c r="D150" s="3">
-        <v>43955</v>
+        <v>43958</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
@@ -4258,7 +4258,7 @@
         <v>NPRO NO Equity</v>
       </c>
       <c r="D151" s="3">
-        <v>43956</v>
+        <v>43959</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
@@ -4273,7 +4273,7 @@
         <v>NRC NO Equity</v>
       </c>
       <c r="D152" s="3">
-        <v>43957</v>
+        <v>43962</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
@@ -4288,7 +4288,7 @@
         <v>NTS NO Equity</v>
       </c>
       <c r="D153" s="3">
-        <v>43958</v>
+        <v>43963</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
@@ -4303,7 +4303,7 @@
         <v>OBSERV NO Equity</v>
       </c>
       <c r="D154" s="3">
-        <v>43959</v>
+        <v>43964</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
@@ -4318,7 +4318,7 @@
         <v>OCY NO Equity</v>
       </c>
       <c r="D155" s="3">
-        <v>43962</v>
+        <v>43965</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
@@ -4333,7 +4333,7 @@
         <v>OTS NO Equity</v>
       </c>
       <c r="D156" s="3">
-        <v>43963</v>
+        <v>43966</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
@@ -4348,7 +4348,7 @@
         <v>ODL NO Equity</v>
       </c>
       <c r="D157" s="3">
-        <v>43964</v>
+        <v>43969</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
@@ -4363,7 +4363,7 @@
         <v>ODF NO Equity</v>
       </c>
       <c r="D158" s="3">
-        <v>43965</v>
+        <v>43970</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
@@ -4378,7 +4378,7 @@
         <v>ODFB NO Equity</v>
       </c>
       <c r="D159" s="3">
-        <v>43966</v>
+        <v>43971</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
@@ -4393,7 +4393,7 @@
         <v>OKEA NO Equity</v>
       </c>
       <c r="D160" s="3">
-        <v>43969</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
@@ -4408,7 +4408,7 @@
         <v>OET NO Equity</v>
       </c>
       <c r="D161" s="3">
-        <v>43970</v>
+        <v>43976</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
@@ -4423,7 +4423,7 @@
         <v>OLT NO Equity</v>
       </c>
       <c r="D162" s="3">
-        <v>43971</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
@@ -4438,7 +4438,7 @@
         <v>ORK NO Equity</v>
       </c>
       <c r="D163" s="3">
-        <v>43972</v>
+        <v>43978</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
@@ -4453,7 +4453,7 @@
         <v>OTELLO NO Equity</v>
       </c>
       <c r="D164" s="3">
-        <v>43973</v>
+        <v>43979</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
@@ -4468,7 +4468,7 @@
         <v>PEN NO Equity</v>
       </c>
       <c r="D165" s="3">
-        <v>43977</v>
+        <v>43980</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
@@ -4483,7 +4483,7 @@
         <v>PARB NO Equity</v>
       </c>
       <c r="D166" s="3">
-        <v>43978</v>
+        <v>43984</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
@@ -4498,7 +4498,7 @@
         <v>PCIB NO Equity</v>
       </c>
       <c r="D167" s="3">
-        <v>43979</v>
+        <v>43985</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
@@ -4513,7 +4513,7 @@
         <v>PSE NO Equity</v>
       </c>
       <c r="D168" s="3">
-        <v>43980</v>
+        <v>43986</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
@@ -4528,7 +4528,7 @@
         <v>PNOR NO Equity</v>
       </c>
       <c r="D169" s="3">
-        <v>43983</v>
+        <v>43987</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
@@ -4543,7 +4543,7 @@
         <v>PEXIP NO Equity</v>
       </c>
       <c r="D170" s="3">
-        <v>43984</v>
+        <v>43990</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
@@ -4558,7 +4558,7 @@
         <v>PGS NO Equity</v>
       </c>
       <c r="D171" s="3">
-        <v>43985</v>
+        <v>43991</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
@@ -4573,7 +4573,7 @@
         <v>PHLY NO Equity</v>
       </c>
       <c r="D172" s="3">
-        <v>43986</v>
+        <v>43992</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
@@ -4588,7 +4588,7 @@
         <v>PHO NO Equity</v>
       </c>
       <c r="D173" s="3">
-        <v>43987</v>
+        <v>43993</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
@@ -4603,7 +4603,7 @@
         <v>PPG PREF NO Equity</v>
       </c>
       <c r="D174" s="3">
-        <v>43990</v>
+        <v>43994</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
@@ -4618,7 +4618,7 @@
         <v>PLCS NO Equity</v>
       </c>
       <c r="D175" s="3">
-        <v>43991</v>
+        <v>43997</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.35">
@@ -4633,7 +4633,7 @@
         <v>POL NO Equity</v>
       </c>
       <c r="D176" s="3">
-        <v>43992</v>
+        <v>43998</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
@@ -4648,7 +4648,7 @@
         <v>PLT NO Equity</v>
       </c>
       <c r="D177" s="3">
-        <v>43993</v>
+        <v>43999</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
@@ -4663,7 +4663,7 @@
         <v>PRS NO Equity</v>
       </c>
       <c r="D178" s="3">
-        <v>43994</v>
+        <v>44000</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
@@ -4678,7 +4678,7 @@
         <v>PROTCT NO Equity</v>
       </c>
       <c r="D179" s="3">
-        <v>43997</v>
+        <v>44001</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
@@ -4693,7 +4693,7 @@
         <v>QFR NO Equity</v>
       </c>
       <c r="D180" s="3">
-        <v>43998</v>
+        <v>44004</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
@@ -4708,7 +4708,7 @@
         <v>QFUELME NO Equity</v>
       </c>
       <c r="D181" s="3">
-        <v>43999</v>
+        <v>44005</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.35">
@@ -4723,7 +4723,7 @@
         <v>QEC NO Equity</v>
       </c>
       <c r="D182" s="3">
-        <v>44000</v>
+        <v>44006</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.35">
@@ -4738,7 +4738,7 @@
         <v>RAKP NO Equity</v>
       </c>
       <c r="D183" s="3">
-        <v>44001</v>
+        <v>44007</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.35">
@@ -4753,7 +4753,7 @@
         <v>REACH NO Equity</v>
       </c>
       <c r="D184" s="3">
-        <v>44004</v>
+        <v>44008</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.35">
@@ -4768,7 +4768,7 @@
         <v>REC NO Equity</v>
       </c>
       <c r="D185" s="3">
-        <v>44005</v>
+        <v>44011</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.35">
@@ -4783,7 +4783,7 @@
         <v>RIVERME NO Equity</v>
       </c>
       <c r="D186" s="3">
-        <v>44006</v>
+        <v>44012</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.35">
@@ -4798,7 +4798,7 @@
         <v>ROM NO Equity</v>
       </c>
       <c r="D187" s="3">
-        <v>44007</v>
+        <v>44013</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.35">
@@ -4813,7 +4813,7 @@
         <v>ROMSBME NO Equity</v>
       </c>
       <c r="D188" s="3">
-        <v>44008</v>
+        <v>44014</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.35">
@@ -4828,7 +4828,7 @@
         <v>SDSD NO Equity</v>
       </c>
       <c r="D189" s="3">
-        <v>44011</v>
+        <v>44015</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.35">
@@ -4843,7 +4843,7 @@
         <v>SAGA NO Equity</v>
       </c>
       <c r="D190" s="3">
-        <v>44012</v>
+        <v>44018</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.35">
@@ -4858,7 +4858,7 @@
         <v>SALM NO Equity</v>
       </c>
       <c r="D191" s="3">
-        <v>44013</v>
+        <v>44019</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.35">
@@ -4873,7 +4873,7 @@
         <v>SALMON NO Equity</v>
       </c>
       <c r="D192" s="3">
-        <v>44014</v>
+        <v>44020</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.35">
@@ -4888,7 +4888,7 @@
         <v>SADG NO Equity</v>
       </c>
       <c r="D193" s="3">
-        <v>44018</v>
+        <v>44021</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.35">
@@ -4903,7 +4903,7 @@
         <v>SAS NOK NO Equity</v>
       </c>
       <c r="D194" s="3">
-        <v>44019</v>
+        <v>44022</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.35">
@@ -4918,7 +4918,7 @@
         <v>SATS NO Equity</v>
       </c>
       <c r="D195" s="3">
-        <v>44020</v>
+        <v>44025</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.35">
@@ -4933,7 +4933,7 @@
         <v>SBANK NO Equity</v>
       </c>
       <c r="D196" s="3">
-        <v>44021</v>
+        <v>44026</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.35">
@@ -4948,7 +4948,7 @@
         <v>SCANA NO Equity</v>
       </c>
       <c r="D197" s="3">
-        <v>44022</v>
+        <v>44027</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.35">
@@ -4963,7 +4963,7 @@
         <v>SSO NO Equity</v>
       </c>
       <c r="D198" s="3">
-        <v>44025</v>
+        <v>44028</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.35">
@@ -4978,7 +4978,7 @@
         <v>SCHA NO Equity</v>
       </c>
       <c r="D199" s="3">
-        <v>44026</v>
+        <v>44029</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.35">
@@ -4993,7 +4993,7 @@
         <v>SCHB NO Equity</v>
       </c>
       <c r="D200" s="3">
-        <v>44027</v>
+        <v>44032</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.35">
@@ -5008,7 +5008,7 @@
         <v>SBX NO Equity</v>
       </c>
       <c r="D201" s="3">
-        <v>44028</v>
+        <v>44033</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.35">
@@ -5023,7 +5023,7 @@
         <v>SDRL NO Equity</v>
       </c>
       <c r="D202" s="3">
-        <v>44029</v>
+        <v>44034</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.35">
@@ -5038,7 +5038,7 @@
         <v>SSG NO Equity</v>
       </c>
       <c r="D203" s="3">
-        <v>44032</v>
+        <v>44035</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.35">
@@ -5053,7 +5053,7 @@
         <v>SBO NO Equity</v>
       </c>
       <c r="D204" s="3">
-        <v>44033</v>
+        <v>44036</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.35">
@@ -5068,7 +5068,7 @@
         <v>SHLF NO Equity</v>
       </c>
       <c r="D205" s="3">
-        <v>44034</v>
+        <v>44039</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.35">
@@ -5083,7 +5083,7 @@
         <v>SIOFF NO Equity</v>
       </c>
       <c r="D206" s="3">
-        <v>44035</v>
+        <v>44040</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.35">
@@ -5098,7 +5098,7 @@
         <v>SIKRIME NO Equity</v>
       </c>
       <c r="D207" s="3">
-        <v>44036</v>
+        <v>44041</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.35">
@@ -5113,7 +5113,7 @@
         <v>SKUE NO Equity</v>
       </c>
       <c r="D208" s="3">
-        <v>44039</v>
+        <v>44042</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.35">
@@ -5128,7 +5128,7 @@
         <v>SOFTOXME NO Equity</v>
       </c>
       <c r="D209" s="3">
-        <v>44040</v>
+        <v>44043</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.35">
@@ -5143,7 +5143,7 @@
         <v>SOGN NO Equity</v>
       </c>
       <c r="D210" s="3">
-        <v>44041</v>
+        <v>44046</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.35">
@@ -5158,7 +5158,7 @@
         <v>SOLON NO Equity</v>
       </c>
       <c r="D211" s="3">
-        <v>44042</v>
+        <v>44047</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.35">
@@ -5173,7 +5173,7 @@
         <v>SOFF NO Equity</v>
       </c>
       <c r="D212" s="3">
-        <v>44043</v>
+        <v>44048</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.35">
@@ -5188,7 +5188,7 @@
         <v>SBVG NO Equity</v>
       </c>
       <c r="D213" s="3">
-        <v>44046</v>
+        <v>44049</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.35">
@@ -5203,7 +5203,7 @@
         <v>NONG NO Equity</v>
       </c>
       <c r="D214" s="3">
-        <v>44047</v>
+        <v>44050</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.35">
@@ -5218,7 +5218,7 @@
         <v>SNOR NO Equity</v>
       </c>
       <c r="D215" s="3">
-        <v>44048</v>
+        <v>44053</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.35">
@@ -5233,7 +5233,7 @@
         <v>RING NO Equity</v>
       </c>
       <c r="D216" s="3">
-        <v>44049</v>
+        <v>44054</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.35">
@@ -5248,7 +5248,7 @@
         <v>MING NO Equity</v>
       </c>
       <c r="D217" s="3">
-        <v>44050</v>
+        <v>44055</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.35">
@@ -5263,7 +5263,7 @@
         <v>SRBANK NO Equity</v>
       </c>
       <c r="D218" s="3">
-        <v>44053</v>
+        <v>44056</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.35">
@@ -5278,7 +5278,7 @@
         <v>SOAG NO Equity</v>
       </c>
       <c r="D219" s="3">
-        <v>44054</v>
+        <v>44057</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.35">
@@ -5293,7 +5293,7 @@
         <v>SPOL NO Equity</v>
       </c>
       <c r="D220" s="3">
-        <v>44055</v>
+        <v>44060</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.35">
@@ -5308,7 +5308,7 @@
         <v>MORG NO Equity</v>
       </c>
       <c r="D221" s="3">
-        <v>44056</v>
+        <v>44061</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.35">
@@ -5323,7 +5323,7 @@
         <v>SOR NO Equity</v>
       </c>
       <c r="D222" s="3">
-        <v>44057</v>
+        <v>44062</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.35">
@@ -5338,7 +5338,7 @@
         <v>SBTE NO Equity</v>
       </c>
       <c r="D223" s="3">
-        <v>44060</v>
+        <v>44063</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.35">
@@ -5353,7 +5353,7 @@
         <v>SVEG NO Equity</v>
       </c>
       <c r="D224" s="3">
-        <v>44061</v>
+        <v>44064</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.35">
@@ -5368,7 +5368,7 @@
         <v>SPOG NO Equity</v>
       </c>
       <c r="D225" s="3">
-        <v>44062</v>
+        <v>44067</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.35">
@@ -5383,7 +5383,7 @@
         <v>SNI NO Equity</v>
       </c>
       <c r="D226" s="3">
-        <v>44063</v>
+        <v>44068</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.35">
@@ -5398,7 +5398,7 @@
         <v>STB NO Equity</v>
       </c>
       <c r="D227" s="3">
-        <v>44064</v>
+        <v>44069</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.35">
@@ -5413,7 +5413,7 @@
         <v>STORM NO Equity</v>
       </c>
       <c r="D228" s="3">
-        <v>44067</v>
+        <v>44070</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.35">
@@ -5428,7 +5428,7 @@
         <v>STRONG NO Equity</v>
       </c>
       <c r="D229" s="3">
-        <v>44068</v>
+        <v>44071</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.35">
@@ -5443,7 +5443,7 @@
         <v>SUBC NO Equity</v>
       </c>
       <c r="D230" s="3">
-        <v>44069</v>
+        <v>44074</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.35">
@@ -5458,7 +5458,7 @@
         <v>SUNSBME NO Equity</v>
       </c>
       <c r="D231" s="3">
-        <v>44070</v>
+        <v>44075</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.35">
@@ -5473,7 +5473,7 @@
         <v>SUSBME NO Equity</v>
       </c>
       <c r="D232" s="3">
-        <v>44071</v>
+        <v>44076</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.35">
@@ -5488,7 +5488,7 @@
         <v>TRVX NO Equity</v>
       </c>
       <c r="D233" s="3">
-        <v>44074</v>
+        <v>44077</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.35">
@@ -5503,7 +5503,7 @@
         <v>TEAM NO Equity</v>
       </c>
       <c r="D234" s="3">
-        <v>44075</v>
+        <v>44078</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.35">
@@ -5518,7 +5518,7 @@
         <v>TECH NO Equity</v>
       </c>
       <c r="D235" s="3">
-        <v>44076</v>
+        <v>44081</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.35">
@@ -5533,7 +5533,7 @@
         <v>TEL NO Equity</v>
       </c>
       <c r="D236" s="3">
-        <v>44077</v>
+        <v>44082</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.35">
@@ -5548,7 +5548,7 @@
         <v>TGS NO Equity</v>
       </c>
       <c r="D237" s="3">
-        <v>44078</v>
+        <v>44083</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.35">
@@ -5563,7 +5563,7 @@
         <v>THIN NO Equity</v>
       </c>
       <c r="D238" s="3">
-        <v>44082</v>
+        <v>44084</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.35">
@@ -5578,7 +5578,7 @@
         <v>TIETOO NO Equity</v>
       </c>
       <c r="D239" s="3">
-        <v>44083</v>
+        <v>44085</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.35">
@@ -5593,7 +5593,7 @@
         <v>TOM NO Equity</v>
       </c>
       <c r="D240" s="3">
-        <v>44084</v>
+        <v>44088</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.35">
@@ -5608,7 +5608,7 @@
         <v>TOTG NO Equity</v>
       </c>
       <c r="D241" s="3">
-        <v>44085</v>
+        <v>44089</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.35">
@@ -5623,7 +5623,7 @@
         <v>TRE NO Equity</v>
       </c>
       <c r="D242" s="3">
-        <v>44088</v>
+        <v>44090</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.35">
@@ -5638,7 +5638,7 @@
         <v>TYSBME NO Equity</v>
       </c>
       <c r="D243" s="3">
-        <v>44089</v>
+        <v>44091</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.35">
@@ -5653,7 +5653,7 @@
         <v>ULTIMO NO Equity</v>
       </c>
       <c r="D244" s="3">
-        <v>44090</v>
+        <v>44092</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.35">
@@ -5668,7 +5668,7 @@
         <v>VEI NO Equity</v>
       </c>
       <c r="D245" s="3">
-        <v>44091</v>
+        <v>44095</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.35">
@@ -5683,7 +5683,7 @@
         <v>VISTIN NO Equity</v>
       </c>
       <c r="D246" s="3">
-        <v>44092</v>
+        <v>44096</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.35">
@@ -5698,7 +5698,7 @@
         <v>VVL NO Equity</v>
       </c>
       <c r="D247" s="3">
-        <v>44095</v>
+        <v>44097</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.35">
@@ -5713,7 +5713,7 @@
         <v>VOW NO Equity</v>
       </c>
       <c r="D248" s="3">
-        <v>44096</v>
+        <v>44098</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.35">
@@ -5728,7 +5728,7 @@
         <v>WALWIL NO Equity</v>
       </c>
       <c r="D249" s="3">
-        <v>44097</v>
+        <v>44099</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.35">
@@ -5743,7 +5743,7 @@
         <v>WSTEP NO Equity</v>
       </c>
       <c r="D250" s="3">
-        <v>44098</v>
+        <v>44102</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.35">
@@ -5758,7 +5758,7 @@
         <v>WWI NO Equity</v>
       </c>
       <c r="D251" s="3">
-        <v>44099</v>
+        <v>44103</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.35">
@@ -5773,7 +5773,7 @@
         <v>WWIB NO Equity</v>
       </c>
       <c r="D252" s="3">
-        <v>44102</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.35">
@@ -5788,7 +5788,7 @@
         <v>WILS NO Equity</v>
       </c>
       <c r="D253" s="3">
-        <v>44103</v>
+        <v>44105</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.35">
@@ -5803,7 +5803,7 @@
         <v>XXL NO Equity</v>
       </c>
       <c r="D254" s="3">
-        <v>44104</v>
+        <v>44106</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.35">
@@ -5818,7 +5818,7 @@
         <v>YAR NO Equity</v>
       </c>
       <c r="D255" s="3">
-        <v>44105</v>
+        <v>44109</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.35">
@@ -5833,7 +5833,7 @@
         <v>ZAL NO Equity</v>
       </c>
       <c r="D256" s="3">
-        <v>44106</v>
+        <v>44110</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.35">
@@ -5848,7 +5848,7 @@
         <v>ZENAME NO Equity</v>
       </c>
       <c r="D257" s="3">
-        <v>44109</v>
+        <v>44111</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.35">
@@ -5863,43 +5863,39 @@
         <v>ZWIPEME NO Equity</v>
       </c>
       <c r="D258" s="3">
-        <v>44110</v>
+        <v>44112</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D259" s="3">
-        <v>44111</v>
+        <v>44113</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D260" s="3">
-        <v>44112</v>
+        <v>44116</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D261" s="3">
-        <v>44113</v>
+        <v>44117</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D262" s="3">
-        <v>44116</v>
+        <v>44118</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D263" s="3">
-        <v>44117</v>
+        <v>44119</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D264" s="3">
-        <v>44118</v>
-      </c>
+      <c r="D264" s="3"/>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D265" s="3">
-        <v>44119</v>
-      </c>
+      <c r="D265" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
updated files to download more variables
</commit_message>
<xml_diff>
--- a/Stock_data/ticker_date.xlsx
+++ b/Stock_data/ticker_date.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Odin Mjølsnes\Documents\myrepo2\Stock_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EBC7B2-CB8B-4E7E-B44B-9545D7EF7773}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC3882D-9C9F-4216-A13E-E3BA0E76CC62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{350AA195-DF91-4F4A-A14B-BEDADCFFE301}"/>
   </bookViews>
@@ -1958,10 +1958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA26B976-9A87-448C-B3C3-776059C9EE67}">
-  <dimension ref="A1:D264"/>
+  <dimension ref="A1:D265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3363,7 +3363,7 @@
         <v>HBC NO Equity</v>
       </c>
       <c r="D93" s="3">
-        <v>43874</v>
+        <v>43873</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
@@ -3378,7 +3378,7 @@
         <v>HUNT NO Equity</v>
       </c>
       <c r="D94" s="3">
-        <v>43875</v>
+        <v>43874</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
@@ -3393,7 +3393,7 @@
         <v>HLNG NO Equity</v>
       </c>
       <c r="D95" s="3">
-        <v>43878</v>
+        <v>43875</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
@@ -3408,7 +3408,7 @@
         <v>HSPG NO Equity</v>
       </c>
       <c r="D96" s="3">
-        <v>43879</v>
+        <v>43878</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
@@ -3423,7 +3423,7 @@
         <v>IFISHME NO Equity</v>
       </c>
       <c r="D97" s="3">
-        <v>43880</v>
+        <v>43879</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
@@ -3438,7 +3438,7 @@
         <v>ICE NO Equity</v>
       </c>
       <c r="D98" s="3">
-        <v>43881</v>
+        <v>43880</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
@@ -3453,7 +3453,7 @@
         <v>IDEX NO Equity</v>
       </c>
       <c r="D99" s="3">
-        <v>43882</v>
+        <v>43881</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
@@ -3468,7 +3468,7 @@
         <v>INDUCTME NO Equity</v>
       </c>
       <c r="D100" s="3">
-        <v>43885</v>
+        <v>43882</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
@@ -3483,7 +3483,7 @@
         <v>INFRNT NO Equity</v>
       </c>
       <c r="D101" s="3">
-        <v>43886</v>
+        <v>43885</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
@@ -3498,7 +3498,7 @@
         <v>INSR NO Equity</v>
       </c>
       <c r="D102" s="3">
-        <v>43887</v>
+        <v>43886</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
@@ -3513,7 +3513,7 @@
         <v>INSTAME NO Equity</v>
       </c>
       <c r="D103" s="3">
-        <v>43888</v>
+        <v>43887</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
@@ -3528,7 +3528,7 @@
         <v>IOX NO Equity</v>
       </c>
       <c r="D104" s="3">
-        <v>43889</v>
+        <v>43888</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
@@ -3543,7 +3543,7 @@
         <v>ITE NO Equity</v>
       </c>
       <c r="D105" s="3">
-        <v>43892</v>
+        <v>43889</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
@@ -3558,7 +3558,7 @@
         <v>JPKME NO Equity</v>
       </c>
       <c r="D106" s="3">
-        <v>43893</v>
+        <v>43892</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
@@ -3573,7 +3573,7 @@
         <v>JIN NO Equity</v>
       </c>
       <c r="D107" s="3">
-        <v>43894</v>
+        <v>43893</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
@@ -3588,7 +3588,7 @@
         <v>JAEREN NO Equity</v>
       </c>
       <c r="D108" s="3">
-        <v>43895</v>
+        <v>43894</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
@@ -3603,7 +3603,7 @@
         <v>KAHOOTME NO Equity</v>
       </c>
       <c r="D109" s="3">
-        <v>43896</v>
+        <v>43895</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
@@ -3618,7 +3618,7 @@
         <v>KID NO Equity</v>
       </c>
       <c r="D110" s="3">
-        <v>43899</v>
+        <v>43896</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
@@ -3633,7 +3633,7 @@
         <v>KIT NO Equity</v>
       </c>
       <c r="D111" s="3">
-        <v>43900</v>
+        <v>43899</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
@@ -3648,7 +3648,7 @@
         <v>KCC NO Equity</v>
       </c>
       <c r="D112" s="3">
-        <v>43901</v>
+        <v>43900</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
@@ -3663,7 +3663,7 @@
         <v>KOMP NO Equity</v>
       </c>
       <c r="D113" s="3">
-        <v>43902</v>
+        <v>43901</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
@@ -3678,7 +3678,7 @@
         <v>KOA NO Equity</v>
       </c>
       <c r="D114" s="3">
-        <v>43903</v>
+        <v>43902</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
@@ -3693,7 +3693,7 @@
         <v>KOG NO Equity</v>
       </c>
       <c r="D115" s="3">
-        <v>43906</v>
+        <v>43903</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
@@ -3708,7 +3708,7 @@
         <v>KVAER NO Equity</v>
       </c>
       <c r="D116" s="3">
-        <v>43907</v>
+        <v>43906</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
@@ -3723,7 +3723,7 @@
         <v>LAVOME NO Equity</v>
       </c>
       <c r="D117" s="3">
-        <v>43908</v>
+        <v>43907</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
@@ -3738,7 +3738,7 @@
         <v>LSG NO Equity</v>
       </c>
       <c r="D118" s="3">
-        <v>43909</v>
+        <v>43908</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
@@ -3753,7 +3753,7 @@
         <v>LIFEME NO Equity</v>
       </c>
       <c r="D119" s="3">
-        <v>43910</v>
+        <v>43909</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
@@ -3768,7 +3768,7 @@
         <v>LSTSBME NO Equity</v>
       </c>
       <c r="D120" s="3">
-        <v>43913</v>
+        <v>43910</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
@@ -3783,7 +3783,7 @@
         <v>MGN NO Equity</v>
       </c>
       <c r="D121" s="3">
-        <v>43914</v>
+        <v>43913</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
@@ -3798,7 +3798,7 @@
         <v>MSEIS NO Equity</v>
       </c>
       <c r="D122" s="3">
-        <v>43915</v>
+        <v>43914</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
@@ -3813,7 +3813,7 @@
         <v>MEDI NO Equity</v>
       </c>
       <c r="D123" s="3">
-        <v>43916</v>
+        <v>43915</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
@@ -3828,7 +3828,7 @@
         <v>MELG NO Equity</v>
       </c>
       <c r="D124" s="3">
-        <v>43917</v>
+        <v>43916</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
@@ -3843,7 +3843,7 @@
         <v>MRCELME NO Equity</v>
       </c>
       <c r="D125" s="3">
-        <v>43920</v>
+        <v>43917</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
@@ -3858,7 +3858,7 @@
         <v>MOWI NO Equity</v>
       </c>
       <c r="D126" s="3">
-        <v>43921</v>
+        <v>43920</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
@@ -3873,7 +3873,7 @@
         <v>MPCC NO Equity</v>
       </c>
       <c r="D127" s="3">
-        <v>43922</v>
+        <v>43921</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
@@ -3888,7 +3888,7 @@
         <v>MULTI NO Equity</v>
       </c>
       <c r="D128" s="3">
-        <v>43923</v>
+        <v>43922</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
@@ -3903,7 +3903,7 @@
         <v>NAPA NO Equity</v>
       </c>
       <c r="D129" s="3">
-        <v>43924</v>
+        <v>43923</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
@@ -3918,7 +3918,7 @@
         <v>NATTO NO Equity</v>
       </c>
       <c r="D130" s="3">
-        <v>43927</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
@@ -3933,7 +3933,7 @@
         <v>NAVA NO Equity</v>
       </c>
       <c r="D131" s="3">
-        <v>43928</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
@@ -3948,7 +3948,7 @@
         <v>NKR NO Equity</v>
       </c>
       <c r="D132" s="3">
-        <v>43929</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
@@ -3963,7 +3963,7 @@
         <v>NEL NO Equity</v>
       </c>
       <c r="D133" s="3">
-        <v>43935</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
@@ -3978,7 +3978,7 @@
         <v>NEXT NO Equity</v>
       </c>
       <c r="D134" s="3">
-        <v>43936</v>
+        <v>43935</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
@@ -3993,7 +3993,7 @@
         <v>NISBME NO Equity</v>
       </c>
       <c r="D135" s="3">
-        <v>43937</v>
+        <v>43936</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
@@ -4008,7 +4008,7 @@
         <v>NORBIT NO Equity</v>
       </c>
       <c r="D136" s="3">
-        <v>43938</v>
+        <v>43937</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
@@ -4023,7 +4023,7 @@
         <v>NOM NO Equity</v>
       </c>
       <c r="D137" s="3">
-        <v>43941</v>
+        <v>43938</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
@@ -4038,7 +4038,7 @@
         <v>NANO NO Equity</v>
       </c>
       <c r="D138" s="3">
-        <v>43942</v>
+        <v>43941</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
@@ -4053,7 +4053,7 @@
         <v>NOD NO Equity</v>
       </c>
       <c r="D139" s="3">
-        <v>43943</v>
+        <v>43942</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
@@ -4068,7 +4068,7 @@
         <v>NHY NO Equity</v>
       </c>
       <c r="D140" s="3">
-        <v>43944</v>
+        <v>43943</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
@@ -4083,7 +4083,7 @@
         <v>NSKOG NO Equity</v>
       </c>
       <c r="D141" s="3">
-        <v>43945</v>
+        <v>43944</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
@@ -4098,7 +4098,7 @@
         <v>NORTH NO Equity</v>
       </c>
       <c r="D142" s="3">
-        <v>43948</v>
+        <v>43945</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
@@ -4113,7 +4113,7 @@
         <v>NODL NO Equity</v>
       </c>
       <c r="D143" s="3">
-        <v>43949</v>
+        <v>43948</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
@@ -4128,7 +4128,7 @@
         <v>NOL NO Equity</v>
       </c>
       <c r="D144" s="3">
-        <v>43950</v>
+        <v>43949</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
@@ -4143,7 +4143,7 @@
         <v>NRS NO Equity</v>
       </c>
       <c r="D145" s="3">
-        <v>43951</v>
+        <v>43950</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
@@ -4158,7 +4158,7 @@
         <v>NAS NO Equity</v>
       </c>
       <c r="D146" s="3">
-        <v>43955</v>
+        <v>43951</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
@@ -4173,7 +4173,7 @@
         <v>NOR NO Equity</v>
       </c>
       <c r="D147" s="3">
-        <v>43956</v>
+        <v>43955</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
@@ -4188,7 +4188,7 @@
         <v>NOFI NO Equity</v>
       </c>
       <c r="D148" s="3">
-        <v>43957</v>
+        <v>43956</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
@@ -4203,7 +4203,7 @@
         <v>NPRO NO Equity</v>
       </c>
       <c r="D149" s="3">
-        <v>43958</v>
+        <v>43957</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
@@ -4218,7 +4218,7 @@
         <v>NRC NO Equity</v>
       </c>
       <c r="D150" s="3">
-        <v>43959</v>
+        <v>43958</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
@@ -4233,7 +4233,7 @@
         <v>NTS NO Equity</v>
       </c>
       <c r="D151" s="3">
-        <v>43962</v>
+        <v>43959</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
@@ -4248,7 +4248,7 @@
         <v>OBSERV NO Equity</v>
       </c>
       <c r="D152" s="3">
-        <v>43963</v>
+        <v>43962</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
@@ -4263,7 +4263,7 @@
         <v>OCY NO Equity</v>
       </c>
       <c r="D153" s="3">
-        <v>43964</v>
+        <v>43963</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
@@ -4278,7 +4278,7 @@
         <v>OTS NO Equity</v>
       </c>
       <c r="D154" s="3">
-        <v>43965</v>
+        <v>43964</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
@@ -4293,7 +4293,7 @@
         <v>ODL NO Equity</v>
       </c>
       <c r="D155" s="3">
-        <v>43966</v>
+        <v>43965</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
@@ -4308,7 +4308,7 @@
         <v>ODF NO Equity</v>
       </c>
       <c r="D156" s="3">
-        <v>43969</v>
+        <v>43966</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
@@ -4323,7 +4323,7 @@
         <v>ODFB NO Equity</v>
       </c>
       <c r="D157" s="3">
-        <v>43970</v>
+        <v>43969</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
@@ -4338,7 +4338,7 @@
         <v>OKEA NO Equity</v>
       </c>
       <c r="D158" s="3">
-        <v>43971</v>
+        <v>43970</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
@@ -4353,7 +4353,7 @@
         <v>OET NO Equity</v>
       </c>
       <c r="D159" s="3">
-        <v>43973</v>
+        <v>43971</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
@@ -4368,7 +4368,7 @@
         <v>OLT NO Equity</v>
       </c>
       <c r="D160" s="3">
-        <v>43976</v>
+        <v>43973</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
@@ -4383,7 +4383,7 @@
         <v>ORK NO Equity</v>
       </c>
       <c r="D161" s="3">
-        <v>43977</v>
+        <v>43976</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
@@ -4398,7 +4398,7 @@
         <v>OTELLO NO Equity</v>
       </c>
       <c r="D162" s="3">
-        <v>43978</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
@@ -4413,7 +4413,7 @@
         <v>PEN NO Equity</v>
       </c>
       <c r="D163" s="3">
-        <v>43979</v>
+        <v>43978</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
@@ -4428,7 +4428,7 @@
         <v>PARB NO Equity</v>
       </c>
       <c r="D164" s="3">
-        <v>43980</v>
+        <v>43979</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
@@ -4443,7 +4443,7 @@
         <v>PCIB NO Equity</v>
       </c>
       <c r="D165" s="3">
-        <v>43984</v>
+        <v>43980</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
@@ -4458,7 +4458,7 @@
         <v>PSE NO Equity</v>
       </c>
       <c r="D166" s="3">
-        <v>43985</v>
+        <v>43984</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
@@ -4473,7 +4473,7 @@
         <v>PNOR NO Equity</v>
       </c>
       <c r="D167" s="3">
-        <v>43986</v>
+        <v>43985</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
@@ -4488,7 +4488,7 @@
         <v>PEXIP NO Equity</v>
       </c>
       <c r="D168" s="3">
-        <v>43987</v>
+        <v>43986</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
@@ -4503,7 +4503,7 @@
         <v>PGS NO Equity</v>
       </c>
       <c r="D169" s="3">
-        <v>43990</v>
+        <v>43987</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
@@ -4518,7 +4518,7 @@
         <v>PHLY NO Equity</v>
       </c>
       <c r="D170" s="3">
-        <v>43991</v>
+        <v>43990</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
@@ -4533,7 +4533,7 @@
         <v>PHO NO Equity</v>
       </c>
       <c r="D171" s="3">
-        <v>43992</v>
+        <v>43991</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
@@ -4548,7 +4548,7 @@
         <v>PPG PREF NO Equity</v>
       </c>
       <c r="D172" s="3">
-        <v>43993</v>
+        <v>43992</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
@@ -4563,7 +4563,7 @@
         <v>PLCS NO Equity</v>
       </c>
       <c r="D173" s="3">
-        <v>43994</v>
+        <v>43993</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
@@ -4578,7 +4578,7 @@
         <v>POL NO Equity</v>
       </c>
       <c r="D174" s="3">
-        <v>43997</v>
+        <v>43994</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
@@ -4593,7 +4593,7 @@
         <v>PLT NO Equity</v>
       </c>
       <c r="D175" s="3">
-        <v>43998</v>
+        <v>43997</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.35">
@@ -4608,7 +4608,7 @@
         <v>PRS NO Equity</v>
       </c>
       <c r="D176" s="3">
-        <v>43999</v>
+        <v>43998</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
@@ -4623,7 +4623,7 @@
         <v>PROTCT NO Equity</v>
       </c>
       <c r="D177" s="3">
-        <v>44000</v>
+        <v>43999</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
@@ -4638,7 +4638,7 @@
         <v>QFR NO Equity</v>
       </c>
       <c r="D178" s="3">
-        <v>44001</v>
+        <v>44000</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
@@ -4653,7 +4653,7 @@
         <v>QFUELME NO Equity</v>
       </c>
       <c r="D179" s="3">
-        <v>44004</v>
+        <v>44001</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
@@ -4668,7 +4668,7 @@
         <v>QEC NO Equity</v>
       </c>
       <c r="D180" s="3">
-        <v>44005</v>
+        <v>44004</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
@@ -4683,7 +4683,7 @@
         <v>RAKP NO Equity</v>
       </c>
       <c r="D181" s="3">
-        <v>44006</v>
+        <v>44005</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.35">
@@ -4698,7 +4698,7 @@
         <v>REACH NO Equity</v>
       </c>
       <c r="D182" s="3">
-        <v>44007</v>
+        <v>44006</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.35">
@@ -4713,7 +4713,7 @@
         <v>REC NO Equity</v>
       </c>
       <c r="D183" s="3">
-        <v>44008</v>
+        <v>44007</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.35">
@@ -4728,7 +4728,7 @@
         <v>RIVERME NO Equity</v>
       </c>
       <c r="D184" s="3">
-        <v>44011</v>
+        <v>44008</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.35">
@@ -4743,7 +4743,7 @@
         <v>ROM NO Equity</v>
       </c>
       <c r="D185" s="3">
-        <v>44012</v>
+        <v>44011</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.35">
@@ -4758,7 +4758,7 @@
         <v>ROMSBME NO Equity</v>
       </c>
       <c r="D186" s="3">
-        <v>44013</v>
+        <v>44012</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.35">
@@ -4773,7 +4773,7 @@
         <v>SDSD NO Equity</v>
       </c>
       <c r="D187" s="3">
-        <v>44014</v>
+        <v>44013</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.35">
@@ -4788,7 +4788,7 @@
         <v>SAGA NO Equity</v>
       </c>
       <c r="D188" s="3">
-        <v>44015</v>
+        <v>44014</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.35">
@@ -4803,7 +4803,7 @@
         <v>SALM NO Equity</v>
       </c>
       <c r="D189" s="3">
-        <v>44018</v>
+        <v>44015</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.35">
@@ -4818,7 +4818,7 @@
         <v>SALMON NO Equity</v>
       </c>
       <c r="D190" s="3">
-        <v>44019</v>
+        <v>44018</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.35">
@@ -4833,7 +4833,7 @@
         <v>SADG NO Equity</v>
       </c>
       <c r="D191" s="3">
-        <v>44020</v>
+        <v>44019</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.35">
@@ -4848,7 +4848,7 @@
         <v>SASNOK NO Equity</v>
       </c>
       <c r="D192" s="3">
-        <v>44021</v>
+        <v>44020</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.35">
@@ -4863,7 +4863,7 @@
         <v>SATS NO Equity</v>
       </c>
       <c r="D193" s="3">
-        <v>44022</v>
+        <v>44021</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.35">
@@ -4878,7 +4878,7 @@
         <v>SBANK NO Equity</v>
       </c>
       <c r="D194" s="3">
-        <v>44025</v>
+        <v>44022</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.35">
@@ -4893,7 +4893,7 @@
         <v>SCANA NO Equity</v>
       </c>
       <c r="D195" s="3">
-        <v>44026</v>
+        <v>44025</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.35">
@@ -4908,7 +4908,7 @@
         <v>SSO NO Equity</v>
       </c>
       <c r="D196" s="3">
-        <v>44027</v>
+        <v>44026</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.35">
@@ -4923,7 +4923,7 @@
         <v>SCHA NO Equity</v>
       </c>
       <c r="D197" s="3">
-        <v>44028</v>
+        <v>44027</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.35">
@@ -4938,7 +4938,7 @@
         <v>SCHB NO Equity</v>
       </c>
       <c r="D198" s="3">
-        <v>44029</v>
+        <v>44028</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.35">
@@ -4953,7 +4953,7 @@
         <v>SBX NO Equity</v>
       </c>
       <c r="D199" s="3">
-        <v>44032</v>
+        <v>44029</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.35">
@@ -4968,7 +4968,7 @@
         <v>SDRL NO Equity</v>
       </c>
       <c r="D200" s="3">
-        <v>44033</v>
+        <v>44032</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.35">
@@ -4983,7 +4983,7 @@
         <v>SSG NO Equity</v>
       </c>
       <c r="D201" s="3">
-        <v>44034</v>
+        <v>44033</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.35">
@@ -4998,7 +4998,7 @@
         <v>SBO NO Equity</v>
       </c>
       <c r="D202" s="3">
-        <v>44035</v>
+        <v>44034</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.35">
@@ -5013,7 +5013,7 @@
         <v>SHLF NO Equity</v>
       </c>
       <c r="D203" s="3">
-        <v>44036</v>
+        <v>44035</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.35">
@@ -5028,7 +5028,7 @@
         <v>SIOFF NO Equity</v>
       </c>
       <c r="D204" s="3">
-        <v>44039</v>
+        <v>44036</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.35">
@@ -5043,7 +5043,7 @@
         <v>SIKRIME NO Equity</v>
       </c>
       <c r="D205" s="3">
-        <v>44040</v>
+        <v>44039</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.35">
@@ -5058,7 +5058,7 @@
         <v>SKUE NO Equity</v>
       </c>
       <c r="D206" s="3">
-        <v>44041</v>
+        <v>44040</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.35">
@@ -5073,7 +5073,7 @@
         <v>SOFTOXME NO Equity</v>
       </c>
       <c r="D207" s="3">
-        <v>44042</v>
+        <v>44041</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.35">
@@ -5088,7 +5088,7 @@
         <v>SOGN NO Equity</v>
       </c>
       <c r="D208" s="3">
-        <v>44043</v>
+        <v>44042</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.35">
@@ -5103,7 +5103,7 @@
         <v>SOLON NO Equity</v>
       </c>
       <c r="D209" s="3">
-        <v>44046</v>
+        <v>44043</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.35">
@@ -5118,7 +5118,7 @@
         <v>SOFF NO Equity</v>
       </c>
       <c r="D210" s="3">
-        <v>44047</v>
+        <v>44046</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.35">
@@ -5133,7 +5133,7 @@
         <v>SBVG NO Equity</v>
       </c>
       <c r="D211" s="3">
-        <v>44048</v>
+        <v>44047</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.35">
@@ -5148,7 +5148,7 @@
         <v>NONG NO Equity</v>
       </c>
       <c r="D212" s="3">
-        <v>44049</v>
+        <v>44048</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.35">
@@ -5163,7 +5163,7 @@
         <v>SNOR NO Equity</v>
       </c>
       <c r="D213" s="3">
-        <v>44050</v>
+        <v>44049</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.35">
@@ -5178,7 +5178,7 @@
         <v>RING NO Equity</v>
       </c>
       <c r="D214" s="3">
-        <v>44053</v>
+        <v>44050</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.35">
@@ -5193,7 +5193,7 @@
         <v>MING NO Equity</v>
       </c>
       <c r="D215" s="3">
-        <v>44054</v>
+        <v>44053</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.35">
@@ -5208,7 +5208,7 @@
         <v>SRBANK NO Equity</v>
       </c>
       <c r="D216" s="3">
-        <v>44055</v>
+        <v>44054</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.35">
@@ -5223,7 +5223,7 @@
         <v>SOAG NO Equity</v>
       </c>
       <c r="D217" s="3">
-        <v>44056</v>
+        <v>44055</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.35">
@@ -5238,7 +5238,7 @@
         <v>SPOL NO Equity</v>
       </c>
       <c r="D218" s="3">
-        <v>44057</v>
+        <v>44056</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.35">
@@ -5253,7 +5253,7 @@
         <v>MORG NO Equity</v>
       </c>
       <c r="D219" s="3">
-        <v>44060</v>
+        <v>44057</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.35">
@@ -5268,7 +5268,7 @@
         <v>SOR NO Equity</v>
       </c>
       <c r="D220" s="3">
-        <v>44061</v>
+        <v>44060</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.35">
@@ -5283,7 +5283,7 @@
         <v>SBTE NO Equity</v>
       </c>
       <c r="D221" s="3">
-        <v>44062</v>
+        <v>44061</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.35">
@@ -5298,7 +5298,7 @@
         <v>SVEG NO Equity</v>
       </c>
       <c r="D222" s="3">
-        <v>44063</v>
+        <v>44062</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.35">
@@ -5313,7 +5313,7 @@
         <v>SPOG NO Equity</v>
       </c>
       <c r="D223" s="3">
-        <v>44064</v>
+        <v>44063</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.35">
@@ -5328,7 +5328,7 @@
         <v>SNI NO Equity</v>
       </c>
       <c r="D224" s="3">
-        <v>44067</v>
+        <v>44064</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.35">
@@ -5343,7 +5343,7 @@
         <v>STB NO Equity</v>
       </c>
       <c r="D225" s="3">
-        <v>44068</v>
+        <v>44067</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.35">
@@ -5358,7 +5358,7 @@
         <v>STORM NO Equity</v>
       </c>
       <c r="D226" s="3">
-        <v>44069</v>
+        <v>44068</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.35">
@@ -5373,7 +5373,7 @@
         <v>STRONG NO Equity</v>
       </c>
       <c r="D227" s="3">
-        <v>44070</v>
+        <v>44069</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.35">
@@ -5388,7 +5388,7 @@
         <v>SUBC NO Equity</v>
       </c>
       <c r="D228" s="3">
-        <v>44071</v>
+        <v>44070</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.35">
@@ -5403,7 +5403,7 @@
         <v>SUNSBME NO Equity</v>
       </c>
       <c r="D229" s="3">
-        <v>44074</v>
+        <v>44071</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.35">
@@ -5418,7 +5418,7 @@
         <v>SUSBME NO Equity</v>
       </c>
       <c r="D230" s="3">
-        <v>44075</v>
+        <v>44074</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.35">
@@ -5433,7 +5433,7 @@
         <v>TRVX NO Equity</v>
       </c>
       <c r="D231" s="3">
-        <v>44076</v>
+        <v>44075</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.35">
@@ -5448,7 +5448,7 @@
         <v>TEAM NO Equity</v>
       </c>
       <c r="D232" s="3">
-        <v>44077</v>
+        <v>44076</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.35">
@@ -5463,7 +5463,7 @@
         <v>TECH NO Equity</v>
       </c>
       <c r="D233" s="3">
-        <v>44078</v>
+        <v>44077</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.35">
@@ -5478,7 +5478,7 @@
         <v>TEL NO Equity</v>
       </c>
       <c r="D234" s="3">
-        <v>44081</v>
+        <v>44078</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.35">
@@ -5493,7 +5493,7 @@
         <v>TGS NO Equity</v>
       </c>
       <c r="D235" s="3">
-        <v>44082</v>
+        <v>44081</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.35">
@@ -5508,7 +5508,7 @@
         <v>THIN NO Equity</v>
       </c>
       <c r="D236" s="3">
-        <v>44083</v>
+        <v>44082</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.35">
@@ -5523,7 +5523,7 @@
         <v>TIETOO NO Equity</v>
       </c>
       <c r="D237" s="3">
-        <v>44084</v>
+        <v>44083</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.35">
@@ -5538,7 +5538,7 @@
         <v>TOM NO Equity</v>
       </c>
       <c r="D238" s="3">
-        <v>44085</v>
+        <v>44084</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.35">
@@ -5553,7 +5553,7 @@
         <v>TOTG NO Equity</v>
       </c>
       <c r="D239" s="3">
-        <v>44088</v>
+        <v>44085</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.35">
@@ -5568,7 +5568,7 @@
         <v>TRE NO Equity</v>
       </c>
       <c r="D240" s="3">
-        <v>44089</v>
+        <v>44088</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.35">
@@ -5583,7 +5583,7 @@
         <v>TYSBME NO Equity</v>
       </c>
       <c r="D241" s="3">
-        <v>44090</v>
+        <v>44089</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.35">
@@ -5598,7 +5598,7 @@
         <v>ULTIMO NO Equity</v>
       </c>
       <c r="D242" s="3">
-        <v>44091</v>
+        <v>44090</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.35">
@@ -5613,7 +5613,7 @@
         <v>VEI NO Equity</v>
       </c>
       <c r="D243" s="3">
-        <v>44092</v>
+        <v>44091</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.35">
@@ -5628,7 +5628,7 @@
         <v>VISTIN NO Equity</v>
       </c>
       <c r="D244" s="3">
-        <v>44095</v>
+        <v>44092</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.35">
@@ -5643,7 +5643,7 @@
         <v>VVL NO Equity</v>
       </c>
       <c r="D245" s="3">
-        <v>44096</v>
+        <v>44095</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.35">
@@ -5658,7 +5658,7 @@
         <v>VOW NO Equity</v>
       </c>
       <c r="D246" s="3">
-        <v>44097</v>
+        <v>44096</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.35">
@@ -5673,7 +5673,7 @@
         <v>WALWIL NO Equity</v>
       </c>
       <c r="D247" s="3">
-        <v>44098</v>
+        <v>44097</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.35">
@@ -5688,7 +5688,7 @@
         <v>WSTEP NO Equity</v>
       </c>
       <c r="D248" s="3">
-        <v>44099</v>
+        <v>44098</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.35">
@@ -5703,7 +5703,7 @@
         <v>WWI NO Equity</v>
       </c>
       <c r="D249" s="3">
-        <v>44102</v>
+        <v>44099</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.35">
@@ -5718,7 +5718,7 @@
         <v>WWIB NO Equity</v>
       </c>
       <c r="D250" s="3">
-        <v>44103</v>
+        <v>44102</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.35">
@@ -5733,7 +5733,7 @@
         <v>WILS NO Equity</v>
       </c>
       <c r="D251" s="3">
-        <v>44104</v>
+        <v>44103</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.35">
@@ -5748,7 +5748,7 @@
         <v>XXL NO Equity</v>
       </c>
       <c r="D252" s="3">
-        <v>44105</v>
+        <v>44104</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.35">
@@ -5763,7 +5763,7 @@
         <v>YAR NO Equity</v>
       </c>
       <c r="D253" s="3">
-        <v>44106</v>
+        <v>44105</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.35">
@@ -5778,7 +5778,7 @@
         <v>ZAL NO Equity</v>
       </c>
       <c r="D254" s="3">
-        <v>44109</v>
+        <v>44106</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.35">
@@ -5793,7 +5793,7 @@
         <v>ZENAME NO Equity</v>
       </c>
       <c r="D255" s="3">
-        <v>44110</v>
+        <v>44109</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.35">
@@ -5808,44 +5808,49 @@
         <v>ZWIPEME NO Equity</v>
       </c>
       <c r="D256" s="3">
-        <v>44111</v>
+        <v>44110</v>
       </c>
     </row>
     <row r="257" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D257" s="3">
-        <v>44112</v>
+        <v>44111</v>
       </c>
     </row>
     <row r="258" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D258" s="3">
-        <v>44113</v>
+        <v>44112</v>
       </c>
     </row>
     <row r="259" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D259" s="3">
-        <v>44116</v>
+        <v>44113</v>
       </c>
     </row>
     <row r="260" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D260" s="3">
-        <v>44117</v>
+        <v>44116</v>
       </c>
     </row>
     <row r="261" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D261" s="3">
-        <v>44118</v>
+        <v>44117</v>
       </c>
     </row>
     <row r="262" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D262" s="3">
+        <v>44118</v>
+      </c>
+    </row>
+    <row r="263" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D263" s="3">
         <v>44119</v>
       </c>
-    </row>
-    <row r="263" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D263" s="3"/>
     </row>
     <row r="264" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D264" s="3"/>
+    </row>
+    <row r="265" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D265" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
updated stock data with expanded date sequence
</commit_message>
<xml_diff>
--- a/Stock_data/ticker_date.xlsx
+++ b/Stock_data/ticker_date.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Odin Mjølsnes\Documents\myrepo2\Stock_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC3882D-9C9F-4216-A13E-E3BA0E76CC62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB8B0F2-ED32-42EE-9E74-3CE16AB7B6F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{350AA195-DF91-4F4A-A14B-BEDADCFFE301}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Cities" sheetId="2" r:id="rId2"/>
-    <sheet name="Repeat" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,30 +32,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="503">
   <si>
     <t>Zwipe</t>
   </si>
@@ -1416,30 +1392,6 @@
   </si>
   <si>
     <t>2020 Bulkers</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>Cities</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
   </si>
   <si>
     <t>AASBME</t>
@@ -1596,16 +1548,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1639,10 +1583,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1958,10 +1900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA26B976-9A87-448C-B3C3-776059C9EE67}">
-  <dimension ref="A1:D265"/>
+  <dimension ref="A1:E294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="G93" sqref="G93"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1970,20 +1912,21 @@
     <col min="2" max="2" width="30.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="B1" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="C1" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="D1" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1997,7 +1940,7 @@
         <f>_xlfn.CONCAT(A2," NO"," Equity")</f>
         <v>2020 NO Equity</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
         <v>43739</v>
       </c>
     </row>
@@ -2012,13 +1955,13 @@
         <f t="shared" ref="C3:C66" si="0">_xlfn.CONCAT(A3," NO"," Equity")</f>
         <v>FIVEPG NO Equity</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
         <v>43740</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="B4" t="s">
         <v>449</v>
@@ -2027,7 +1970,7 @@
         <f t="shared" si="0"/>
         <v>AASBME NO Equity</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
         <v>43741</v>
       </c>
     </row>
@@ -2042,7 +1985,7 @@
         <f t="shared" si="0"/>
         <v>ASC NO Equity</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>43742</v>
       </c>
     </row>
@@ -2057,13 +2000,13 @@
         <f t="shared" si="0"/>
         <v>ADE NO Equity</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="1">
         <v>43745</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="B7" t="s">
         <v>444</v>
@@ -2072,7 +2015,7 @@
         <f t="shared" si="0"/>
         <v>ADSCME NO Equity</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="1">
         <v>43746</v>
       </c>
     </row>
@@ -2087,7 +2030,7 @@
         <f t="shared" si="0"/>
         <v>AEGA NO Equity</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="1">
         <v>43747</v>
       </c>
     </row>
@@ -2102,7 +2045,7 @@
         <f t="shared" si="0"/>
         <v>AFG NO Equity</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="1">
         <v>43748</v>
       </c>
     </row>
@@ -2117,7 +2060,7 @@
         <f t="shared" si="0"/>
         <v>AKA NO Equity</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="1">
         <v>43749</v>
       </c>
     </row>
@@ -2132,13 +2075,13 @@
         <f t="shared" si="0"/>
         <v>AKER NO Equity</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="1">
         <v>43752</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="B12" t="s">
         <v>435</v>
@@ -2147,7 +2090,7 @@
         <f t="shared" si="0"/>
         <v>AKBMME NO Equity</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="1">
         <v>43753</v>
       </c>
     </row>
@@ -2162,13 +2105,13 @@
         <f t="shared" si="0"/>
         <v>AKERBP NO Equity</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="1">
         <v>43754</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="B14" t="s">
         <v>432</v>
@@ -2177,13 +2120,13 @@
         <f t="shared" si="0"/>
         <v>ACCME NO Equity</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="1">
         <v>43755</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="B15" t="s">
         <v>431</v>
@@ -2192,7 +2135,7 @@
         <f t="shared" si="0"/>
         <v>AOWME NO Equity</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="1">
         <v>43756</v>
       </c>
     </row>
@@ -2207,7 +2150,7 @@
         <f t="shared" si="0"/>
         <v>AKSO NO Equity</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="1">
         <v>43759</v>
       </c>
     </row>
@@ -2222,7 +2165,7 @@
         <f t="shared" si="0"/>
         <v>AKVA NO Equity</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="1">
         <v>43760</v>
       </c>
     </row>
@@ -2237,13 +2180,13 @@
         <f t="shared" si="0"/>
         <v>AMSC NO Equity</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="1">
         <v>43761</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="B19" t="s">
         <v>424</v>
@@ -2252,7 +2195,7 @@
         <f t="shared" si="0"/>
         <v>ANDFME NO Equity</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="1">
         <v>43762</v>
       </c>
     </row>
@@ -2267,7 +2210,7 @@
         <f t="shared" si="0"/>
         <v>ABT NO Equity</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="1">
         <v>43763</v>
       </c>
     </row>
@@ -2282,7 +2225,7 @@
         <f t="shared" si="0"/>
         <v>AQUA NO Equity</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="1">
         <v>43766</v>
       </c>
     </row>
@@ -2297,7 +2240,7 @@
         <f t="shared" si="0"/>
         <v>ARCHER NO Equity</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="1">
         <v>43767</v>
       </c>
     </row>
@@ -2312,7 +2255,7 @@
         <f t="shared" si="0"/>
         <v>AZT NO Equity</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="1">
         <v>43768</v>
       </c>
     </row>
@@ -2327,7 +2270,7 @@
         <f t="shared" si="0"/>
         <v>ARCUS NO Equity</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="1">
         <v>43769</v>
       </c>
     </row>
@@ -2342,7 +2285,7 @@
         <f t="shared" si="0"/>
         <v>AFK NO Equity</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="1">
         <v>43770</v>
       </c>
     </row>
@@ -2357,7 +2300,7 @@
         <f t="shared" si="0"/>
         <v>ASETEK NO Equity</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="1">
         <v>43773</v>
       </c>
     </row>
@@ -2372,13 +2315,13 @@
         <f t="shared" si="0"/>
         <v>ATEA NO Equity</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="1">
         <v>43774</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="B28" t="s">
         <v>407</v>
@@ -2387,7 +2330,7 @@
         <f t="shared" si="0"/>
         <v>ATLA NO Equity</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="1">
         <v>43775</v>
       </c>
     </row>
@@ -2402,7 +2345,7 @@
         <f t="shared" si="0"/>
         <v>ASA NO Equity</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="1">
         <v>43776</v>
       </c>
     </row>
@@ -2417,7 +2360,7 @@
         <f t="shared" si="0"/>
         <v>AURG NO Equity</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="1">
         <v>43777</v>
       </c>
     </row>
@@ -2432,7 +2375,7 @@
         <f t="shared" si="0"/>
         <v>AUSS NO Equity</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="1">
         <v>43780</v>
       </c>
     </row>
@@ -2447,7 +2390,7 @@
         <f t="shared" si="0"/>
         <v>AVANCE NO Equity</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="1">
         <v>43781</v>
       </c>
     </row>
@@ -2462,7 +2405,7 @@
         <f t="shared" si="0"/>
         <v>AWDR NO Equity</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="1">
         <v>43782</v>
       </c>
     </row>
@@ -2477,7 +2420,7 @@
         <f t="shared" si="0"/>
         <v>ALNG NO Equity</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="1">
         <v>43783</v>
       </c>
     </row>
@@ -2492,7 +2435,7 @@
         <f t="shared" si="0"/>
         <v>AXA NO Equity</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="1">
         <v>43784</v>
       </c>
     </row>
@@ -2507,13 +2450,13 @@
         <f t="shared" si="0"/>
         <v>AGS NO Equity</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="1">
         <v>43787</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="B37" t="s">
         <v>390</v>
@@ -2522,7 +2465,7 @@
         <f t="shared" si="0"/>
         <v>AYFIEME NO Equity</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="1">
         <v>43788</v>
       </c>
     </row>
@@ -2537,7 +2480,7 @@
         <f t="shared" si="0"/>
         <v>B2H NO Equity</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="1">
         <v>43789</v>
       </c>
     </row>
@@ -2552,13 +2495,13 @@
         <f t="shared" si="0"/>
         <v>BAKKA NO Equity</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="1">
         <v>43790</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="B40" t="s">
         <v>385</v>
@@ -2567,7 +2510,7 @@
         <f t="shared" si="0"/>
         <v>BALTME NO Equity</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="1">
         <v>43791</v>
       </c>
     </row>
@@ -2582,7 +2525,7 @@
         <f t="shared" si="0"/>
         <v>BEL NO Equity</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="1">
         <v>43794</v>
       </c>
     </row>
@@ -2597,13 +2540,13 @@
         <f t="shared" si="0"/>
         <v>BGBIO NO Equity</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="1">
         <v>43795</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="B43" t="s">
         <v>380</v>
@@ -2612,13 +2555,13 @@
         <f t="shared" si="0"/>
         <v>BEWIME NO Equity</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="1">
         <v>43796</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="B44" t="s">
         <v>379</v>
@@ -2627,7 +2570,7 @@
         <f t="shared" si="0"/>
         <v>BSPME NO Equity</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="1">
         <v>43797</v>
       </c>
     </row>
@@ -2642,7 +2585,7 @@
         <f t="shared" si="0"/>
         <v>BON NO Equity</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="1">
         <v>43798</v>
       </c>
     </row>
@@ -2657,7 +2600,7 @@
         <f t="shared" si="0"/>
         <v>BOR NO Equity</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="1">
         <v>43801</v>
       </c>
     </row>
@@ -2672,7 +2615,7 @@
         <f t="shared" si="0"/>
         <v>BDRILL NO Equity</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="1">
         <v>43802</v>
       </c>
     </row>
@@ -2687,7 +2630,7 @@
         <f t="shared" si="0"/>
         <v>BRG NO Equity</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="1">
         <v>43803</v>
       </c>
     </row>
@@ -2702,13 +2645,13 @@
         <f t="shared" si="0"/>
         <v>BOUVET NO Equity</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="1">
         <v>43804</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="B50" t="s">
         <v>368</v>
@@ -2717,7 +2660,7 @@
         <f t="shared" si="0"/>
         <v>BRAME NO Equity</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="1">
         <v>43805</v>
       </c>
     </row>
@@ -2732,7 +2675,7 @@
         <f t="shared" si="0"/>
         <v>BWE NO Equity</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="1">
         <v>43808</v>
       </c>
     </row>
@@ -2747,7 +2690,7 @@
         <f t="shared" si="0"/>
         <v>BWLPG NO Equity</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="1">
         <v>43809</v>
       </c>
     </row>
@@ -2762,7 +2705,7 @@
         <f t="shared" si="0"/>
         <v>BWO NO Equity</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="1">
         <v>43810</v>
       </c>
     </row>
@@ -2777,7 +2720,7 @@
         <f t="shared" si="0"/>
         <v>BMA NO Equity</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="1">
         <v>43811</v>
       </c>
     </row>
@@ -2792,13 +2735,13 @@
         <f t="shared" si="0"/>
         <v>CARA NO Equity</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="1">
         <v>43812</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="B56" t="s">
         <v>357</v>
@@ -2807,7 +2750,7 @@
         <f t="shared" si="0"/>
         <v>CLOUDME NO Equity</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="1">
         <v>43815</v>
       </c>
     </row>
@@ -2822,7 +2765,7 @@
         <f t="shared" si="0"/>
         <v>COV NO Equity</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="1">
         <v>43816</v>
       </c>
     </row>
@@ -2837,7 +2780,7 @@
         <f t="shared" si="0"/>
         <v>CRAYON NO Equity</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D58" s="1">
         <v>43817</v>
       </c>
     </row>
@@ -2852,7 +2795,7 @@
         <f t="shared" si="0"/>
         <v>DNB NO Equity</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="1">
         <v>43818</v>
       </c>
     </row>
@@ -2867,7 +2810,7 @@
         <f t="shared" si="0"/>
         <v>DNO NO Equity</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="1">
         <v>43819</v>
       </c>
     </row>
@@ -2882,7 +2825,7 @@
         <f t="shared" si="0"/>
         <v>DOF NO Equity</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="1">
         <v>43822</v>
       </c>
     </row>
@@ -2897,7 +2840,7 @@
         <f t="shared" si="0"/>
         <v>EAM NO Equity</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D62" s="1">
         <v>43826</v>
       </c>
     </row>
@@ -2912,7 +2855,7 @@
         <f t="shared" si="0"/>
         <v>EIOF NO Equity</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="1">
         <v>43829</v>
       </c>
     </row>
@@ -2927,7 +2870,7 @@
         <f t="shared" si="0"/>
         <v>EMGS NO Equity</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="1">
         <v>43832</v>
       </c>
     </row>
@@ -2942,7 +2885,7 @@
         <f t="shared" si="0"/>
         <v>ELE NO Equity</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D65" s="1">
         <v>43833</v>
       </c>
     </row>
@@ -2957,13 +2900,13 @@
         <f t="shared" si="0"/>
         <v>ELK NO Equity</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D66" s="1">
         <v>43836</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="B67" t="s">
         <v>339</v>
@@ -2972,7 +2915,7 @@
         <f t="shared" ref="C67:C128" si="1">_xlfn.CONCAT(A67," NO"," Equity")</f>
         <v>ELOPME NO Equity</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="1">
         <v>43837</v>
       </c>
     </row>
@@ -2987,7 +2930,7 @@
         <f t="shared" si="1"/>
         <v>ENDUR NO Equity</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D68" s="1">
         <v>43838</v>
       </c>
     </row>
@@ -3002,13 +2945,13 @@
         <f t="shared" si="1"/>
         <v>ENTRA NO Equity</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D69" s="1">
         <v>43839</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="B70" t="s">
         <v>334</v>
@@ -3017,7 +2960,7 @@
         <f t="shared" si="1"/>
         <v>EPICME NO Equity</v>
       </c>
-      <c r="D70" s="3">
+      <c r="D70" s="1">
         <v>43840</v>
       </c>
     </row>
@@ -3032,7 +2975,7 @@
         <f t="shared" si="1"/>
         <v>EQNR NO Equity</v>
       </c>
-      <c r="D71" s="3">
+      <c r="D71" s="1">
         <v>43843</v>
       </c>
     </row>
@@ -3047,13 +2990,13 @@
         <f t="shared" si="1"/>
         <v>EPR NO Equity</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D72" s="1">
         <v>43844</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="B73" t="s">
         <v>329</v>
@@ -3062,7 +3005,7 @@
         <f t="shared" si="1"/>
         <v>EXTXME NO Equity</v>
       </c>
-      <c r="D73" s="3">
+      <c r="D73" s="1">
         <v>43845</v>
       </c>
     </row>
@@ -3077,7 +3020,7 @@
         <f t="shared" si="1"/>
         <v>FJORD NO Equity</v>
       </c>
-      <c r="D74" s="3">
+      <c r="D74" s="1">
         <v>43846</v>
       </c>
     </row>
@@ -3092,7 +3035,7 @@
         <f t="shared" si="1"/>
         <v>FKRAFT NO Equity</v>
       </c>
-      <c r="D75" s="3">
+      <c r="D75" s="1">
         <v>43847</v>
       </c>
     </row>
@@ -3107,7 +3050,7 @@
         <f t="shared" si="1"/>
         <v>FLNG NO Equity</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D76" s="1">
         <v>43850</v>
       </c>
     </row>
@@ -3122,7 +3065,7 @@
         <f t="shared" si="1"/>
         <v>FRO NO Equity</v>
       </c>
-      <c r="D77" s="3">
+      <c r="D77" s="1">
         <v>43851</v>
       </c>
     </row>
@@ -3137,7 +3080,7 @@
         <f t="shared" si="1"/>
         <v>GIG NO Equity</v>
       </c>
-      <c r="D78" s="3">
+      <c r="D78" s="1">
         <v>43852</v>
       </c>
     </row>
@@ -3152,13 +3095,13 @@
         <f t="shared" si="1"/>
         <v>RISH NO Equity</v>
       </c>
-      <c r="D79" s="3">
+      <c r="D79" s="1">
         <v>43853</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="B80" t="s">
         <v>316</v>
@@ -3167,7 +3110,7 @@
         <f t="shared" si="1"/>
         <v>GENTME NO Equity</v>
       </c>
-      <c r="D80" s="3">
+      <c r="D80" s="1">
         <v>43854</v>
       </c>
     </row>
@@ -3182,13 +3125,13 @@
         <f t="shared" si="1"/>
         <v>GJF NO Equity</v>
       </c>
-      <c r="D81" s="3">
+      <c r="D81" s="1">
         <v>43857</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="B82" t="s">
         <v>313</v>
@@ -3197,7 +3140,7 @@
         <f t="shared" si="1"/>
         <v>GEOSME NO Equity</v>
       </c>
-      <c r="D82" s="3">
+      <c r="D82" s="1">
         <v>43858</v>
       </c>
     </row>
@@ -3212,7 +3155,7 @@
         <f t="shared" si="1"/>
         <v>GOGL NO Equity</v>
       </c>
-      <c r="D83" s="3">
+      <c r="D83" s="1">
         <v>43859</v>
       </c>
     </row>
@@ -3227,7 +3170,7 @@
         <f t="shared" si="1"/>
         <v>GOD NO Equity</v>
       </c>
-      <c r="D84" s="3">
+      <c r="D84" s="1">
         <v>43860</v>
       </c>
     </row>
@@ -3242,13 +3185,13 @@
         <f t="shared" si="1"/>
         <v>GSF NO Equity</v>
       </c>
-      <c r="D85" s="3">
+      <c r="D85" s="1">
         <v>43861</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="B86" t="s">
         <v>306</v>
@@ -3257,7 +3200,7 @@
         <f t="shared" si="1"/>
         <v>GRONGME NO Equity</v>
       </c>
-      <c r="D86" s="3">
+      <c r="D86" s="1">
         <v>43864</v>
       </c>
     </row>
@@ -3272,7 +3215,7 @@
         <f t="shared" si="1"/>
         <v>GYL NO Equity</v>
       </c>
-      <c r="D87" s="3">
+      <c r="D87" s="1">
         <v>43865</v>
       </c>
     </row>
@@ -3287,7 +3230,7 @@
         <f t="shared" si="1"/>
         <v>HAFNIA NO Equity</v>
       </c>
-      <c r="D88" s="3">
+      <c r="D88" s="1">
         <v>43866</v>
       </c>
     </row>
@@ -3302,7 +3245,7 @@
         <f t="shared" si="1"/>
         <v>HAVI NO Equity</v>
       </c>
-      <c r="D89" s="3">
+      <c r="D89" s="1">
         <v>43867</v>
       </c>
     </row>
@@ -3317,7 +3260,7 @@
         <f t="shared" si="1"/>
         <v>HYARD NO Equity</v>
       </c>
-      <c r="D90" s="3">
+      <c r="D90" s="1">
         <v>43868</v>
       </c>
     </row>
@@ -3332,7 +3275,7 @@
         <f t="shared" si="1"/>
         <v>HELG NO Equity</v>
       </c>
-      <c r="D91" s="3">
+      <c r="D91" s="1">
         <v>43871</v>
       </c>
     </row>
@@ -3347,7 +3290,7 @@
         <f t="shared" si="1"/>
         <v>HEX NO Equity</v>
       </c>
-      <c r="D92" s="3">
+      <c r="D92" s="1">
         <v>43872</v>
       </c>
     </row>
@@ -3362,7 +3305,7 @@
         <f t="shared" si="1"/>
         <v>HBC NO Equity</v>
       </c>
-      <c r="D93" s="3">
+      <c r="D93" s="1">
         <v>43873</v>
       </c>
     </row>
@@ -3377,7 +3320,7 @@
         <f t="shared" si="1"/>
         <v>HUNT NO Equity</v>
       </c>
-      <c r="D94" s="3">
+      <c r="D94" s="1">
         <v>43874</v>
       </c>
     </row>
@@ -3392,7 +3335,7 @@
         <f t="shared" si="1"/>
         <v>HLNG NO Equity</v>
       </c>
-      <c r="D95" s="3">
+      <c r="D95" s="1">
         <v>43875</v>
       </c>
     </row>
@@ -3407,13 +3350,13 @@
         <f t="shared" si="1"/>
         <v>HSPG NO Equity</v>
       </c>
-      <c r="D96" s="3">
+      <c r="D96" s="1">
         <v>43878</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="B97" t="s">
         <v>285</v>
@@ -3422,7 +3365,7 @@
         <f t="shared" si="1"/>
         <v>IFISHME NO Equity</v>
       </c>
-      <c r="D97" s="3">
+      <c r="D97" s="1">
         <v>43879</v>
       </c>
     </row>
@@ -3437,7 +3380,7 @@
         <f t="shared" si="1"/>
         <v>ICE NO Equity</v>
       </c>
-      <c r="D98" s="3">
+      <c r="D98" s="1">
         <v>43880</v>
       </c>
     </row>
@@ -3452,13 +3395,13 @@
         <f t="shared" si="1"/>
         <v>IDEX NO Equity</v>
       </c>
-      <c r="D99" s="3">
+      <c r="D99" s="1">
         <v>43881</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="B100" t="s">
         <v>280</v>
@@ -3467,7 +3410,7 @@
         <f t="shared" si="1"/>
         <v>INDUCTME NO Equity</v>
       </c>
-      <c r="D100" s="3">
+      <c r="D100" s="1">
         <v>43882</v>
       </c>
     </row>
@@ -3482,7 +3425,7 @@
         <f t="shared" si="1"/>
         <v>INFRNT NO Equity</v>
       </c>
-      <c r="D101" s="3">
+      <c r="D101" s="1">
         <v>43885</v>
       </c>
     </row>
@@ -3497,13 +3440,13 @@
         <f t="shared" si="1"/>
         <v>INSR NO Equity</v>
       </c>
-      <c r="D102" s="3">
+      <c r="D102" s="1">
         <v>43886</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="B103" t="s">
         <v>275</v>
@@ -3512,7 +3455,7 @@
         <f t="shared" si="1"/>
         <v>INSTAME NO Equity</v>
       </c>
-      <c r="D103" s="3">
+      <c r="D103" s="1">
         <v>43887</v>
       </c>
     </row>
@@ -3527,7 +3470,7 @@
         <f t="shared" si="1"/>
         <v>IOX NO Equity</v>
       </c>
-      <c r="D104" s="3">
+      <c r="D104" s="1">
         <v>43888</v>
       </c>
     </row>
@@ -3542,13 +3485,13 @@
         <f t="shared" si="1"/>
         <v>ITE NO Equity</v>
       </c>
-      <c r="D105" s="3">
+      <c r="D105" s="1">
         <v>43889</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="B106" t="s">
         <v>270</v>
@@ -3557,7 +3500,7 @@
         <f t="shared" si="1"/>
         <v>JPKME NO Equity</v>
       </c>
-      <c r="D106" s="3">
+      <c r="D106" s="1">
         <v>43892</v>
       </c>
     </row>
@@ -3572,7 +3515,7 @@
         <f t="shared" si="1"/>
         <v>JIN NO Equity</v>
       </c>
-      <c r="D107" s="3">
+      <c r="D107" s="1">
         <v>43893</v>
       </c>
     </row>
@@ -3587,13 +3530,13 @@
         <f t="shared" si="1"/>
         <v>JAEREN NO Equity</v>
       </c>
-      <c r="D108" s="3">
+      <c r="D108" s="1">
         <v>43894</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="B109" t="s">
         <v>265</v>
@@ -3602,7 +3545,7 @@
         <f t="shared" si="1"/>
         <v>KAHOOTME NO Equity</v>
       </c>
-      <c r="D109" s="3">
+      <c r="D109" s="1">
         <v>43895</v>
       </c>
     </row>
@@ -3617,7 +3560,7 @@
         <f t="shared" si="1"/>
         <v>KID NO Equity</v>
       </c>
-      <c r="D110" s="3">
+      <c r="D110" s="1">
         <v>43896</v>
       </c>
     </row>
@@ -3632,7 +3575,7 @@
         <f t="shared" si="1"/>
         <v>KIT NO Equity</v>
       </c>
-      <c r="D111" s="3">
+      <c r="D111" s="1">
         <v>43899</v>
       </c>
     </row>
@@ -3647,7 +3590,7 @@
         <f t="shared" si="1"/>
         <v>KCC NO Equity</v>
       </c>
-      <c r="D112" s="3">
+      <c r="D112" s="1">
         <v>43900</v>
       </c>
     </row>
@@ -3662,7 +3605,7 @@
         <f t="shared" si="1"/>
         <v>KOMP NO Equity</v>
       </c>
-      <c r="D113" s="3">
+      <c r="D113" s="1">
         <v>43901</v>
       </c>
     </row>
@@ -3677,7 +3620,7 @@
         <f t="shared" si="1"/>
         <v>KOA NO Equity</v>
       </c>
-      <c r="D114" s="3">
+      <c r="D114" s="1">
         <v>43902</v>
       </c>
     </row>
@@ -3692,7 +3635,7 @@
         <f t="shared" si="1"/>
         <v>KOG NO Equity</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D115" s="1">
         <v>43903</v>
       </c>
     </row>
@@ -3707,13 +3650,13 @@
         <f t="shared" si="1"/>
         <v>KVAER NO Equity</v>
       </c>
-      <c r="D116" s="3">
+      <c r="D116" s="1">
         <v>43906</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="B117" t="s">
         <v>250</v>
@@ -3722,7 +3665,7 @@
         <f t="shared" si="1"/>
         <v>LAVOME NO Equity</v>
       </c>
-      <c r="D117" s="3">
+      <c r="D117" s="1">
         <v>43907</v>
       </c>
     </row>
@@ -3737,13 +3680,13 @@
         <f t="shared" si="1"/>
         <v>LSG NO Equity</v>
       </c>
-      <c r="D118" s="3">
+      <c r="D118" s="1">
         <v>43908</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="B119" t="s">
         <v>247</v>
@@ -3752,13 +3695,13 @@
         <f t="shared" si="1"/>
         <v>LIFEME NO Equity</v>
       </c>
-      <c r="D119" s="3">
+      <c r="D119" s="1">
         <v>43909</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="B120" t="s">
         <v>246</v>
@@ -3767,7 +3710,7 @@
         <f t="shared" si="1"/>
         <v>LSTSBME NO Equity</v>
       </c>
-      <c r="D120" s="3">
+      <c r="D120" s="1">
         <v>43910</v>
       </c>
     </row>
@@ -3782,7 +3725,7 @@
         <f t="shared" si="1"/>
         <v>MGN NO Equity</v>
       </c>
-      <c r="D121" s="3">
+      <c r="D121" s="1">
         <v>43913</v>
       </c>
     </row>
@@ -3797,7 +3740,7 @@
         <f t="shared" si="1"/>
         <v>MSEIS NO Equity</v>
       </c>
-      <c r="D122" s="3">
+      <c r="D122" s="1">
         <v>43914</v>
       </c>
     </row>
@@ -3812,7 +3755,7 @@
         <f t="shared" si="1"/>
         <v>MEDI NO Equity</v>
       </c>
-      <c r="D123" s="3">
+      <c r="D123" s="1">
         <v>43915</v>
       </c>
     </row>
@@ -3827,13 +3770,13 @@
         <f t="shared" si="1"/>
         <v>MELG NO Equity</v>
       </c>
-      <c r="D124" s="3">
+      <c r="D124" s="1">
         <v>43916</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="B125" t="s">
         <v>237</v>
@@ -3842,7 +3785,7 @@
         <f t="shared" si="1"/>
         <v>MRCELME NO Equity</v>
       </c>
-      <c r="D125" s="3">
+      <c r="D125" s="1">
         <v>43917</v>
       </c>
     </row>
@@ -3857,7 +3800,7 @@
         <f t="shared" si="1"/>
         <v>MOWI NO Equity</v>
       </c>
-      <c r="D126" s="3">
+      <c r="D126" s="1">
         <v>43920</v>
       </c>
     </row>
@@ -3872,7 +3815,7 @@
         <f t="shared" si="1"/>
         <v>MPCC NO Equity</v>
       </c>
-      <c r="D127" s="3">
+      <c r="D127" s="1">
         <v>43921</v>
       </c>
     </row>
@@ -3887,7 +3830,7 @@
         <f t="shared" si="1"/>
         <v>MULTI NO Equity</v>
       </c>
-      <c r="D128" s="3">
+      <c r="D128" s="1">
         <v>43922</v>
       </c>
     </row>
@@ -3902,7 +3845,7 @@
         <f t="shared" ref="C129:C192" si="2">_xlfn.CONCAT(A129," NO"," Equity")</f>
         <v>NAPA NO Equity</v>
       </c>
-      <c r="D129" s="3">
+      <c r="D129" s="1">
         <v>43923</v>
       </c>
     </row>
@@ -3917,7 +3860,7 @@
         <f t="shared" si="2"/>
         <v>NATTO NO Equity</v>
       </c>
-      <c r="D130" s="3">
+      <c r="D130" s="1">
         <v>43924</v>
       </c>
     </row>
@@ -3932,7 +3875,7 @@
         <f t="shared" si="2"/>
         <v>NAVA NO Equity</v>
       </c>
-      <c r="D131" s="3">
+      <c r="D131" s="1">
         <v>43927</v>
       </c>
     </row>
@@ -3947,7 +3890,7 @@
         <f t="shared" si="2"/>
         <v>NKR NO Equity</v>
       </c>
-      <c r="D132" s="3">
+      <c r="D132" s="1">
         <v>43928</v>
       </c>
     </row>
@@ -3962,7 +3905,7 @@
         <f t="shared" si="2"/>
         <v>NEL NO Equity</v>
       </c>
-      <c r="D133" s="3">
+      <c r="D133" s="1">
         <v>43929</v>
       </c>
     </row>
@@ -3977,13 +3920,13 @@
         <f t="shared" si="2"/>
         <v>NEXT NO Equity</v>
       </c>
-      <c r="D134" s="3">
+      <c r="D134" s="1">
         <v>43935</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="B135" t="s">
         <v>219</v>
@@ -3992,7 +3935,7 @@
         <f t="shared" si="2"/>
         <v>NISBME NO Equity</v>
       </c>
-      <c r="D135" s="3">
+      <c r="D135" s="1">
         <v>43936</v>
       </c>
     </row>
@@ -4007,7 +3950,7 @@
         <f t="shared" si="2"/>
         <v>NORBIT NO Equity</v>
       </c>
-      <c r="D136" s="3">
+      <c r="D136" s="1">
         <v>43937</v>
       </c>
     </row>
@@ -4022,7 +3965,7 @@
         <f t="shared" si="2"/>
         <v>NOM NO Equity</v>
       </c>
-      <c r="D137" s="3">
+      <c r="D137" s="1">
         <v>43938</v>
       </c>
     </row>
@@ -4037,7 +3980,7 @@
         <f t="shared" si="2"/>
         <v>NANO NO Equity</v>
       </c>
-      <c r="D138" s="3">
+      <c r="D138" s="1">
         <v>43941</v>
       </c>
     </row>
@@ -4052,7 +3995,7 @@
         <f t="shared" si="2"/>
         <v>NOD NO Equity</v>
       </c>
-      <c r="D139" s="3">
+      <c r="D139" s="1">
         <v>43942</v>
       </c>
     </row>
@@ -4067,7 +4010,7 @@
         <f t="shared" si="2"/>
         <v>NHY NO Equity</v>
       </c>
-      <c r="D140" s="3">
+      <c r="D140" s="1">
         <v>43943</v>
       </c>
     </row>
@@ -4082,7 +4025,7 @@
         <f t="shared" si="2"/>
         <v>NSKOG NO Equity</v>
       </c>
-      <c r="D141" s="3">
+      <c r="D141" s="1">
         <v>43944</v>
       </c>
     </row>
@@ -4097,7 +4040,7 @@
         <f t="shared" si="2"/>
         <v>NORTH NO Equity</v>
       </c>
-      <c r="D142" s="3">
+      <c r="D142" s="1">
         <v>43945</v>
       </c>
     </row>
@@ -4112,7 +4055,7 @@
         <f t="shared" si="2"/>
         <v>NODL NO Equity</v>
       </c>
-      <c r="D143" s="3">
+      <c r="D143" s="1">
         <v>43948</v>
       </c>
     </row>
@@ -4127,7 +4070,7 @@
         <f t="shared" si="2"/>
         <v>NOL NO Equity</v>
       </c>
-      <c r="D144" s="3">
+      <c r="D144" s="1">
         <v>43949</v>
       </c>
     </row>
@@ -4142,7 +4085,7 @@
         <f t="shared" si="2"/>
         <v>NRS NO Equity</v>
       </c>
-      <c r="D145" s="3">
+      <c r="D145" s="1">
         <v>43950</v>
       </c>
     </row>
@@ -4157,7 +4100,7 @@
         <f t="shared" si="2"/>
         <v>NAS NO Equity</v>
       </c>
-      <c r="D146" s="3">
+      <c r="D146" s="1">
         <v>43951</v>
       </c>
     </row>
@@ -4172,7 +4115,7 @@
         <f t="shared" si="2"/>
         <v>NOR NO Equity</v>
       </c>
-      <c r="D147" s="3">
+      <c r="D147" s="1">
         <v>43955</v>
       </c>
     </row>
@@ -4187,7 +4130,7 @@
         <f t="shared" si="2"/>
         <v>NOFI NO Equity</v>
       </c>
-      <c r="D148" s="3">
+      <c r="D148" s="1">
         <v>43956</v>
       </c>
     </row>
@@ -4202,7 +4145,7 @@
         <f t="shared" si="2"/>
         <v>NPRO NO Equity</v>
       </c>
-      <c r="D149" s="3">
+      <c r="D149" s="1">
         <v>43957</v>
       </c>
     </row>
@@ -4217,7 +4160,7 @@
         <f t="shared" si="2"/>
         <v>NRC NO Equity</v>
       </c>
-      <c r="D150" s="3">
+      <c r="D150" s="1">
         <v>43958</v>
       </c>
     </row>
@@ -4232,7 +4175,7 @@
         <f t="shared" si="2"/>
         <v>NTS NO Equity</v>
       </c>
-      <c r="D151" s="3">
+      <c r="D151" s="1">
         <v>43959</v>
       </c>
     </row>
@@ -4247,7 +4190,7 @@
         <f t="shared" si="2"/>
         <v>OBSERV NO Equity</v>
       </c>
-      <c r="D152" s="3">
+      <c r="D152" s="1">
         <v>43962</v>
       </c>
     </row>
@@ -4262,7 +4205,7 @@
         <f t="shared" si="2"/>
         <v>OCY NO Equity</v>
       </c>
-      <c r="D153" s="3">
+      <c r="D153" s="1">
         <v>43963</v>
       </c>
     </row>
@@ -4277,7 +4220,7 @@
         <f t="shared" si="2"/>
         <v>OTS NO Equity</v>
       </c>
-      <c r="D154" s="3">
+      <c r="D154" s="1">
         <v>43964</v>
       </c>
     </row>
@@ -4292,7 +4235,7 @@
         <f t="shared" si="2"/>
         <v>ODL NO Equity</v>
       </c>
-      <c r="D155" s="3">
+      <c r="D155" s="1">
         <v>43965</v>
       </c>
     </row>
@@ -4307,7 +4250,7 @@
         <f t="shared" si="2"/>
         <v>ODF NO Equity</v>
       </c>
-      <c r="D156" s="3">
+      <c r="D156" s="1">
         <v>43966</v>
       </c>
     </row>
@@ -4322,7 +4265,7 @@
         <f t="shared" si="2"/>
         <v>ODFB NO Equity</v>
       </c>
-      <c r="D157" s="3">
+      <c r="D157" s="1">
         <v>43969</v>
       </c>
     </row>
@@ -4337,7 +4280,7 @@
         <f t="shared" si="2"/>
         <v>OKEA NO Equity</v>
       </c>
-      <c r="D158" s="3">
+      <c r="D158" s="1">
         <v>43970</v>
       </c>
     </row>
@@ -4352,7 +4295,7 @@
         <f t="shared" si="2"/>
         <v>OET NO Equity</v>
       </c>
-      <c r="D159" s="3">
+      <c r="D159" s="1">
         <v>43971</v>
       </c>
     </row>
@@ -4367,7 +4310,7 @@
         <f t="shared" si="2"/>
         <v>OLT NO Equity</v>
       </c>
-      <c r="D160" s="3">
+      <c r="D160" s="1">
         <v>43973</v>
       </c>
     </row>
@@ -4382,7 +4325,7 @@
         <f t="shared" si="2"/>
         <v>ORK NO Equity</v>
       </c>
-      <c r="D161" s="3">
+      <c r="D161" s="1">
         <v>43976</v>
       </c>
     </row>
@@ -4397,7 +4340,7 @@
         <f t="shared" si="2"/>
         <v>OTELLO NO Equity</v>
       </c>
-      <c r="D162" s="3">
+      <c r="D162" s="1">
         <v>43977</v>
       </c>
     </row>
@@ -4412,7 +4355,7 @@
         <f t="shared" si="2"/>
         <v>PEN NO Equity</v>
       </c>
-      <c r="D163" s="3">
+      <c r="D163" s="1">
         <v>43978</v>
       </c>
     </row>
@@ -4427,7 +4370,7 @@
         <f t="shared" si="2"/>
         <v>PARB NO Equity</v>
       </c>
-      <c r="D164" s="3">
+      <c r="D164" s="1">
         <v>43979</v>
       </c>
     </row>
@@ -4442,7 +4385,7 @@
         <f t="shared" si="2"/>
         <v>PCIB NO Equity</v>
       </c>
-      <c r="D165" s="3">
+      <c r="D165" s="1">
         <v>43980</v>
       </c>
     </row>
@@ -4457,7 +4400,7 @@
         <f t="shared" si="2"/>
         <v>PSE NO Equity</v>
       </c>
-      <c r="D166" s="3">
+      <c r="D166" s="1">
         <v>43984</v>
       </c>
     </row>
@@ -4472,7 +4415,7 @@
         <f t="shared" si="2"/>
         <v>PNOR NO Equity</v>
       </c>
-      <c r="D167" s="3">
+      <c r="D167" s="1">
         <v>43985</v>
       </c>
     </row>
@@ -4487,7 +4430,7 @@
         <f t="shared" si="2"/>
         <v>PEXIP NO Equity</v>
       </c>
-      <c r="D168" s="3">
+      <c r="D168" s="1">
         <v>43986</v>
       </c>
     </row>
@@ -4502,7 +4445,7 @@
         <f t="shared" si="2"/>
         <v>PGS NO Equity</v>
       </c>
-      <c r="D169" s="3">
+      <c r="D169" s="1">
         <v>43987</v>
       </c>
     </row>
@@ -4517,7 +4460,7 @@
         <f t="shared" si="2"/>
         <v>PHLY NO Equity</v>
       </c>
-      <c r="D170" s="3">
+      <c r="D170" s="1">
         <v>43990</v>
       </c>
     </row>
@@ -4532,7 +4475,7 @@
         <f t="shared" si="2"/>
         <v>PHO NO Equity</v>
       </c>
-      <c r="D171" s="3">
+      <c r="D171" s="1">
         <v>43991</v>
       </c>
     </row>
@@ -4547,7 +4490,7 @@
         <f t="shared" si="2"/>
         <v>PPG PREF NO Equity</v>
       </c>
-      <c r="D172" s="3">
+      <c r="D172" s="1">
         <v>43992</v>
       </c>
     </row>
@@ -4562,7 +4505,7 @@
         <f t="shared" si="2"/>
         <v>PLCS NO Equity</v>
       </c>
-      <c r="D173" s="3">
+      <c r="D173" s="1">
         <v>43993</v>
       </c>
     </row>
@@ -4577,7 +4520,7 @@
         <f t="shared" si="2"/>
         <v>POL NO Equity</v>
       </c>
-      <c r="D174" s="3">
+      <c r="D174" s="1">
         <v>43994</v>
       </c>
     </row>
@@ -4592,7 +4535,7 @@
         <f t="shared" si="2"/>
         <v>PLT NO Equity</v>
       </c>
-      <c r="D175" s="3">
+      <c r="D175" s="1">
         <v>43997</v>
       </c>
     </row>
@@ -4607,7 +4550,7 @@
         <f t="shared" si="2"/>
         <v>PRS NO Equity</v>
       </c>
-      <c r="D176" s="3">
+      <c r="D176" s="1">
         <v>43998</v>
       </c>
     </row>
@@ -4622,7 +4565,7 @@
         <f t="shared" si="2"/>
         <v>PROTCT NO Equity</v>
       </c>
-      <c r="D177" s="3">
+      <c r="D177" s="1">
         <v>43999</v>
       </c>
     </row>
@@ -4631,19 +4574,19 @@
         <v>138</v>
       </c>
       <c r="B178" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="C178" t="str">
         <f t="shared" si="2"/>
         <v>QFR NO Equity</v>
       </c>
-      <c r="D178" s="3">
+      <c r="D178" s="1">
         <v>44000</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="B179" t="s">
         <v>137</v>
@@ -4652,7 +4595,7 @@
         <f t="shared" si="2"/>
         <v>QFUELME NO Equity</v>
       </c>
-      <c r="D179" s="3">
+      <c r="D179" s="1">
         <v>44001</v>
       </c>
     </row>
@@ -4667,7 +4610,7 @@
         <f t="shared" si="2"/>
         <v>QEC NO Equity</v>
       </c>
-      <c r="D180" s="3">
+      <c r="D180" s="1">
         <v>44004</v>
       </c>
     </row>
@@ -4682,7 +4625,7 @@
         <f t="shared" si="2"/>
         <v>RAKP NO Equity</v>
       </c>
-      <c r="D181" s="3">
+      <c r="D181" s="1">
         <v>44005</v>
       </c>
     </row>
@@ -4697,7 +4640,7 @@
         <f t="shared" si="2"/>
         <v>REACH NO Equity</v>
       </c>
-      <c r="D182" s="3">
+      <c r="D182" s="1">
         <v>44006</v>
       </c>
     </row>
@@ -4712,13 +4655,13 @@
         <f t="shared" si="2"/>
         <v>REC NO Equity</v>
       </c>
-      <c r="D183" s="3">
+      <c r="D183" s="1">
         <v>44007</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="B184" t="s">
         <v>128</v>
@@ -4727,7 +4670,7 @@
         <f t="shared" si="2"/>
         <v>RIVERME NO Equity</v>
       </c>
-      <c r="D184" s="3">
+      <c r="D184" s="1">
         <v>44008</v>
       </c>
     </row>
@@ -4742,13 +4685,13 @@
         <f t="shared" si="2"/>
         <v>ROM NO Equity</v>
       </c>
-      <c r="D185" s="3">
+      <c r="D185" s="1">
         <v>44011</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="B186" t="s">
         <v>125</v>
@@ -4757,7 +4700,7 @@
         <f t="shared" si="2"/>
         <v>ROMSBME NO Equity</v>
       </c>
-      <c r="D186" s="3">
+      <c r="D186" s="1">
         <v>44012</v>
       </c>
     </row>
@@ -4772,7 +4715,7 @@
         <f t="shared" si="2"/>
         <v>SDSD NO Equity</v>
       </c>
-      <c r="D187" s="3">
+      <c r="D187" s="1">
         <v>44013</v>
       </c>
     </row>
@@ -4787,7 +4730,7 @@
         <f t="shared" si="2"/>
         <v>SAGA NO Equity</v>
       </c>
-      <c r="D188" s="3">
+      <c r="D188" s="1">
         <v>44014</v>
       </c>
     </row>
@@ -4802,7 +4745,7 @@
         <f t="shared" si="2"/>
         <v>SALM NO Equity</v>
       </c>
-      <c r="D189" s="3">
+      <c r="D189" s="1">
         <v>44015</v>
       </c>
     </row>
@@ -4817,7 +4760,7 @@
         <f t="shared" si="2"/>
         <v>SALMON NO Equity</v>
       </c>
-      <c r="D190" s="3">
+      <c r="D190" s="1">
         <v>44018</v>
       </c>
     </row>
@@ -4832,13 +4775,13 @@
         <f t="shared" si="2"/>
         <v>SADG NO Equity</v>
       </c>
-      <c r="D191" s="3">
+      <c r="D191" s="1">
         <v>44019</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="B192" t="s">
         <v>114</v>
@@ -4847,7 +4790,7 @@
         <f t="shared" si="2"/>
         <v>SASNOK NO Equity</v>
       </c>
-      <c r="D192" s="3">
+      <c r="D192" s="1">
         <v>44020</v>
       </c>
     </row>
@@ -4862,7 +4805,7 @@
         <f t="shared" ref="C193:C256" si="3">_xlfn.CONCAT(A193," NO"," Equity")</f>
         <v>SATS NO Equity</v>
       </c>
-      <c r="D193" s="3">
+      <c r="D193" s="1">
         <v>44021</v>
       </c>
     </row>
@@ -4877,7 +4820,7 @@
         <f t="shared" si="3"/>
         <v>SBANK NO Equity</v>
       </c>
-      <c r="D194" s="3">
+      <c r="D194" s="1">
         <v>44022</v>
       </c>
     </row>
@@ -4892,7 +4835,7 @@
         <f t="shared" si="3"/>
         <v>SCANA NO Equity</v>
       </c>
-      <c r="D195" s="3">
+      <c r="D195" s="1">
         <v>44025</v>
       </c>
     </row>
@@ -4907,7 +4850,7 @@
         <f t="shared" si="3"/>
         <v>SSO NO Equity</v>
       </c>
-      <c r="D196" s="3">
+      <c r="D196" s="1">
         <v>44026</v>
       </c>
     </row>
@@ -4922,7 +4865,7 @@
         <f t="shared" si="3"/>
         <v>SCHA NO Equity</v>
       </c>
-      <c r="D197" s="3">
+      <c r="D197" s="1">
         <v>44027</v>
       </c>
     </row>
@@ -4937,7 +4880,7 @@
         <f t="shared" si="3"/>
         <v>SCHB NO Equity</v>
       </c>
-      <c r="D198" s="3">
+      <c r="D198" s="1">
         <v>44028</v>
       </c>
     </row>
@@ -4952,7 +4895,7 @@
         <f t="shared" si="3"/>
         <v>SBX NO Equity</v>
       </c>
-      <c r="D199" s="3">
+      <c r="D199" s="1">
         <v>44029</v>
       </c>
     </row>
@@ -4967,7 +4910,7 @@
         <f t="shared" si="3"/>
         <v>SDRL NO Equity</v>
       </c>
-      <c r="D200" s="3">
+      <c r="D200" s="1">
         <v>44032</v>
       </c>
     </row>
@@ -4982,7 +4925,7 @@
         <f t="shared" si="3"/>
         <v>SSG NO Equity</v>
       </c>
-      <c r="D201" s="3">
+      <c r="D201" s="1">
         <v>44033</v>
       </c>
     </row>
@@ -4997,7 +4940,7 @@
         <f t="shared" si="3"/>
         <v>SBO NO Equity</v>
       </c>
-      <c r="D202" s="3">
+      <c r="D202" s="1">
         <v>44034</v>
       </c>
     </row>
@@ -5012,7 +4955,7 @@
         <f t="shared" si="3"/>
         <v>SHLF NO Equity</v>
       </c>
-      <c r="D203" s="3">
+      <c r="D203" s="1">
         <v>44035</v>
       </c>
     </row>
@@ -5027,13 +4970,13 @@
         <f t="shared" si="3"/>
         <v>SIOFF NO Equity</v>
       </c>
-      <c r="D204" s="3">
+      <c r="D204" s="1">
         <v>44036</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="B205" t="s">
         <v>90</v>
@@ -5042,7 +4985,7 @@
         <f t="shared" si="3"/>
         <v>SIKRIME NO Equity</v>
       </c>
-      <c r="D205" s="3">
+      <c r="D205" s="1">
         <v>44039</v>
       </c>
     </row>
@@ -5057,13 +5000,13 @@
         <f t="shared" si="3"/>
         <v>SKUE NO Equity</v>
       </c>
-      <c r="D206" s="3">
+      <c r="D206" s="1">
         <v>44040</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B207" t="s">
         <v>87</v>
@@ -5072,7 +5015,7 @@
         <f t="shared" si="3"/>
         <v>SOFTOXME NO Equity</v>
       </c>
-      <c r="D207" s="3">
+      <c r="D207" s="1">
         <v>44041</v>
       </c>
     </row>
@@ -5087,7 +5030,7 @@
         <f t="shared" si="3"/>
         <v>SOGN NO Equity</v>
       </c>
-      <c r="D208" s="3">
+      <c r="D208" s="1">
         <v>44042</v>
       </c>
     </row>
@@ -5102,7 +5045,7 @@
         <f t="shared" si="3"/>
         <v>SOLON NO Equity</v>
       </c>
-      <c r="D209" s="3">
+      <c r="D209" s="1">
         <v>44043</v>
       </c>
     </row>
@@ -5117,7 +5060,7 @@
         <f t="shared" si="3"/>
         <v>SOFF NO Equity</v>
       </c>
-      <c r="D210" s="3">
+      <c r="D210" s="1">
         <v>44046</v>
       </c>
     </row>
@@ -5132,7 +5075,7 @@
         <f t="shared" si="3"/>
         <v>SBVG NO Equity</v>
       </c>
-      <c r="D211" s="3">
+      <c r="D211" s="1">
         <v>44047</v>
       </c>
     </row>
@@ -5141,13 +5084,13 @@
         <v>78</v>
       </c>
       <c r="B212" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="C212" t="str">
         <f t="shared" si="3"/>
         <v>NONG NO Equity</v>
       </c>
-      <c r="D212" s="3">
+      <c r="D212" s="1">
         <v>44048</v>
       </c>
     </row>
@@ -5162,7 +5105,7 @@
         <f t="shared" si="3"/>
         <v>SNOR NO Equity</v>
       </c>
-      <c r="D213" s="3">
+      <c r="D213" s="1">
         <v>44049</v>
       </c>
     </row>
@@ -5177,7 +5120,7 @@
         <f t="shared" si="3"/>
         <v>RING NO Equity</v>
       </c>
-      <c r="D214" s="3">
+      <c r="D214" s="1">
         <v>44050</v>
       </c>
     </row>
@@ -5192,7 +5135,7 @@
         <f t="shared" si="3"/>
         <v>MING NO Equity</v>
       </c>
-      <c r="D215" s="3">
+      <c r="D215" s="1">
         <v>44053</v>
       </c>
     </row>
@@ -5201,13 +5144,13 @@
         <v>71</v>
       </c>
       <c r="B216" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="C216" t="str">
         <f t="shared" si="3"/>
         <v>SRBANK NO Equity</v>
       </c>
-      <c r="D216" s="3">
+      <c r="D216" s="1">
         <v>44054</v>
       </c>
     </row>
@@ -5222,7 +5165,7 @@
         <f t="shared" si="3"/>
         <v>SOAG NO Equity</v>
       </c>
-      <c r="D217" s="3">
+      <c r="D217" s="1">
         <v>44055</v>
       </c>
     </row>
@@ -5237,7 +5180,7 @@
         <f t="shared" si="3"/>
         <v>SPOL NO Equity</v>
       </c>
-      <c r="D218" s="3">
+      <c r="D218" s="1">
         <v>44056</v>
       </c>
     </row>
@@ -5252,7 +5195,7 @@
         <f t="shared" si="3"/>
         <v>MORG NO Equity</v>
       </c>
-      <c r="D219" s="3">
+      <c r="D219" s="1">
         <v>44057</v>
       </c>
     </row>
@@ -5267,7 +5210,7 @@
         <f t="shared" si="3"/>
         <v>SOR NO Equity</v>
       </c>
-      <c r="D220" s="3">
+      <c r="D220" s="1">
         <v>44060</v>
       </c>
     </row>
@@ -5282,7 +5225,7 @@
         <f t="shared" si="3"/>
         <v>SBTE NO Equity</v>
       </c>
-      <c r="D221" s="3">
+      <c r="D221" s="1">
         <v>44061</v>
       </c>
     </row>
@@ -5297,7 +5240,7 @@
         <f t="shared" si="3"/>
         <v>SVEG NO Equity</v>
       </c>
-      <c r="D222" s="3">
+      <c r="D222" s="1">
         <v>44062</v>
       </c>
     </row>
@@ -5312,7 +5255,7 @@
         <f t="shared" si="3"/>
         <v>SPOG NO Equity</v>
       </c>
-      <c r="D223" s="3">
+      <c r="D223" s="1">
         <v>44063</v>
       </c>
     </row>
@@ -5321,13 +5264,13 @@
         <v>56</v>
       </c>
       <c r="B224" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="C224" t="str">
         <f t="shared" si="3"/>
         <v>SNI NO Equity</v>
       </c>
-      <c r="D224" s="3">
+      <c r="D224" s="1">
         <v>44064</v>
       </c>
     </row>
@@ -5342,7 +5285,7 @@
         <f t="shared" si="3"/>
         <v>STB NO Equity</v>
       </c>
-      <c r="D225" s="3">
+      <c r="D225" s="1">
         <v>44067</v>
       </c>
     </row>
@@ -5357,7 +5300,7 @@
         <f t="shared" si="3"/>
         <v>STORM NO Equity</v>
       </c>
-      <c r="D226" s="3">
+      <c r="D226" s="1">
         <v>44068</v>
       </c>
     </row>
@@ -5372,7 +5315,7 @@
         <f t="shared" si="3"/>
         <v>STRONG NO Equity</v>
       </c>
-      <c r="D227" s="3">
+      <c r="D227" s="1">
         <v>44069</v>
       </c>
     </row>
@@ -5387,13 +5330,13 @@
         <f t="shared" si="3"/>
         <v>SUBC NO Equity</v>
       </c>
-      <c r="D228" s="3">
+      <c r="D228" s="1">
         <v>44070</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="B229" t="s">
         <v>47</v>
@@ -5402,13 +5345,13 @@
         <f t="shared" si="3"/>
         <v>SUNSBME NO Equity</v>
       </c>
-      <c r="D229" s="3">
+      <c r="D229" s="1">
         <v>44071</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="B230" t="s">
         <v>46</v>
@@ -5417,7 +5360,7 @@
         <f t="shared" si="3"/>
         <v>SUSBME NO Equity</v>
       </c>
-      <c r="D230" s="3">
+      <c r="D230" s="1">
         <v>44074</v>
       </c>
     </row>
@@ -5432,7 +5375,7 @@
         <f t="shared" si="3"/>
         <v>TRVX NO Equity</v>
       </c>
-      <c r="D231" s="3">
+      <c r="D231" s="1">
         <v>44075</v>
       </c>
     </row>
@@ -5447,7 +5390,7 @@
         <f t="shared" si="3"/>
         <v>TEAM NO Equity</v>
       </c>
-      <c r="D232" s="3">
+      <c r="D232" s="1">
         <v>44076</v>
       </c>
     </row>
@@ -5462,7 +5405,7 @@
         <f t="shared" si="3"/>
         <v>TECH NO Equity</v>
       </c>
-      <c r="D233" s="3">
+      <c r="D233" s="1">
         <v>44077</v>
       </c>
     </row>
@@ -5477,7 +5420,7 @@
         <f t="shared" si="3"/>
         <v>TEL NO Equity</v>
       </c>
-      <c r="D234" s="3">
+      <c r="D234" s="1">
         <v>44078</v>
       </c>
     </row>
@@ -5486,13 +5429,13 @@
         <v>37</v>
       </c>
       <c r="B235" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="C235" t="str">
         <f t="shared" si="3"/>
         <v>TGS NO Equity</v>
       </c>
-      <c r="D235" s="3">
+      <c r="D235" s="1">
         <v>44081</v>
       </c>
     </row>
@@ -5507,7 +5450,7 @@
         <f t="shared" si="3"/>
         <v>THIN NO Equity</v>
       </c>
-      <c r="D236" s="3">
+      <c r="D236" s="1">
         <v>44082</v>
       </c>
     </row>
@@ -5522,7 +5465,7 @@
         <f t="shared" si="3"/>
         <v>TIETOO NO Equity</v>
       </c>
-      <c r="D237" s="3">
+      <c r="D237" s="1">
         <v>44083</v>
       </c>
     </row>
@@ -5537,7 +5480,7 @@
         <f t="shared" si="3"/>
         <v>TOM NO Equity</v>
       </c>
-      <c r="D238" s="3">
+      <c r="D238" s="1">
         <v>44084</v>
       </c>
     </row>
@@ -5552,7 +5495,7 @@
         <f t="shared" si="3"/>
         <v>TOTG NO Equity</v>
       </c>
-      <c r="D239" s="3">
+      <c r="D239" s="1">
         <v>44085</v>
       </c>
     </row>
@@ -5567,13 +5510,13 @@
         <f t="shared" si="3"/>
         <v>TRE NO Equity</v>
       </c>
-      <c r="D240" s="3">
+      <c r="D240" s="1">
         <v>44088</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="B241" t="s">
         <v>26</v>
@@ -5582,7 +5525,7 @@
         <f t="shared" si="3"/>
         <v>TYSBME NO Equity</v>
       </c>
-      <c r="D241" s="3">
+      <c r="D241" s="1">
         <v>44089</v>
       </c>
     </row>
@@ -5597,7 +5540,7 @@
         <f t="shared" si="3"/>
         <v>ULTIMO NO Equity</v>
       </c>
-      <c r="D242" s="3">
+      <c r="D242" s="1">
         <v>44090</v>
       </c>
     </row>
@@ -5612,7 +5555,7 @@
         <f t="shared" si="3"/>
         <v>VEI NO Equity</v>
       </c>
-      <c r="D243" s="3">
+      <c r="D243" s="1">
         <v>44091</v>
       </c>
     </row>
@@ -5627,7 +5570,7 @@
         <f t="shared" si="3"/>
         <v>VISTIN NO Equity</v>
       </c>
-      <c r="D244" s="3">
+      <c r="D244" s="1">
         <v>44092</v>
       </c>
     </row>
@@ -5636,13 +5579,13 @@
         <v>19</v>
       </c>
       <c r="B245" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="C245" t="str">
         <f t="shared" si="3"/>
         <v>VVL NO Equity</v>
       </c>
-      <c r="D245" s="3">
+      <c r="D245" s="1">
         <v>44095</v>
       </c>
     </row>
@@ -5657,7 +5600,7 @@
         <f t="shared" si="3"/>
         <v>VOW NO Equity</v>
       </c>
-      <c r="D246" s="3">
+      <c r="D246" s="1">
         <v>44096</v>
       </c>
     </row>
@@ -5672,7 +5615,7 @@
         <f t="shared" si="3"/>
         <v>WALWIL NO Equity</v>
       </c>
-      <c r="D247" s="3">
+      <c r="D247" s="1">
         <v>44097</v>
       </c>
     </row>
@@ -5687,7 +5630,7 @@
         <f t="shared" si="3"/>
         <v>WSTEP NO Equity</v>
       </c>
-      <c r="D248" s="3">
+      <c r="D248" s="1">
         <v>44098</v>
       </c>
     </row>
@@ -5702,7 +5645,7 @@
         <f t="shared" si="3"/>
         <v>WWI NO Equity</v>
       </c>
-      <c r="D249" s="3">
+      <c r="D249" s="1">
         <v>44099</v>
       </c>
     </row>
@@ -5717,7 +5660,7 @@
         <f t="shared" si="3"/>
         <v>WWIB NO Equity</v>
       </c>
-      <c r="D250" s="3">
+      <c r="D250" s="1">
         <v>44102</v>
       </c>
     </row>
@@ -5732,7 +5675,7 @@
         <f t="shared" si="3"/>
         <v>WILS NO Equity</v>
       </c>
-      <c r="D251" s="3">
+      <c r="D251" s="1">
         <v>44103</v>
       </c>
     </row>
@@ -5747,7 +5690,7 @@
         <f t="shared" si="3"/>
         <v>XXL NO Equity</v>
       </c>
-      <c r="D252" s="3">
+      <c r="D252" s="1">
         <v>44104</v>
       </c>
     </row>
@@ -5762,7 +5705,7 @@
         <f t="shared" si="3"/>
         <v>YAR NO Equity</v>
       </c>
-      <c r="D253" s="3">
+      <c r="D253" s="1">
         <v>44105</v>
       </c>
     </row>
@@ -5777,13 +5720,13 @@
         <f t="shared" si="3"/>
         <v>ZAL NO Equity</v>
       </c>
-      <c r="D254" s="3">
+      <c r="D254" s="1">
         <v>44106</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="B255" t="s">
         <v>1</v>
@@ -5792,13 +5735,13 @@
         <f t="shared" si="3"/>
         <v>ZENAME NO Equity</v>
       </c>
-      <c r="D255" s="3">
+      <c r="D255" s="1">
         <v>44109</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="B256" t="s">
         <v>0</v>
@@ -5807,231 +5750,200 @@
         <f t="shared" si="3"/>
         <v>ZWIPEME NO Equity</v>
       </c>
-      <c r="D256" s="3">
+      <c r="D256" s="1">
         <v>44110</v>
       </c>
     </row>
     <row r="257" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D257" s="3">
+      <c r="D257" s="1">
         <v>44111</v>
       </c>
     </row>
     <row r="258" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D258" s="3">
+      <c r="D258" s="1">
         <v>44112</v>
       </c>
     </row>
     <row r="259" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D259" s="3">
+      <c r="D259" s="1">
         <v>44113</v>
       </c>
     </row>
     <row r="260" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D260" s="3">
+      <c r="D260" s="1">
         <v>44116</v>
       </c>
     </row>
     <row r="261" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D261" s="3">
+      <c r="D261" s="1">
         <v>44117</v>
       </c>
     </row>
     <row r="262" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D262" s="3">
+      <c r="D262" s="1">
         <v>44118</v>
       </c>
     </row>
     <row r="263" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D263" s="3">
+      <c r="D263" s="1">
         <v>44119</v>
       </c>
     </row>
     <row r="264" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D264" s="3"/>
+      <c r="D264" s="1">
+        <v>44120</v>
+      </c>
     </row>
     <row r="265" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D265" s="3"/>
+      <c r="D265" s="1">
+        <v>44123</v>
+      </c>
+    </row>
+    <row r="266" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D266" s="1">
+        <v>44124</v>
+      </c>
+    </row>
+    <row r="267" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D267" s="1">
+        <v>44125</v>
+      </c>
+    </row>
+    <row r="268" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D268" s="1">
+        <v>44126</v>
+      </c>
+    </row>
+    <row r="269" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D269" s="1">
+        <v>44127</v>
+      </c>
+    </row>
+    <row r="270" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D270" s="1">
+        <v>44130</v>
+      </c>
+    </row>
+    <row r="271" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D271" s="1">
+        <v>44131</v>
+      </c>
+    </row>
+    <row r="272" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D272" s="1">
+        <v>44132</v>
+      </c>
+    </row>
+    <row r="273" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D273" s="1">
+        <v>44133</v>
+      </c>
+    </row>
+    <row r="274" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D274" s="1">
+        <v>44134</v>
+      </c>
+    </row>
+    <row r="275" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D275" s="1">
+        <v>44137</v>
+      </c>
+    </row>
+    <row r="276" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D276" s="1">
+        <v>44138</v>
+      </c>
+    </row>
+    <row r="277" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D277" s="1">
+        <v>44139</v>
+      </c>
+    </row>
+    <row r="278" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D278" s="1">
+        <v>44140</v>
+      </c>
+    </row>
+    <row r="279" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D279" s="1">
+        <v>44141</v>
+      </c>
+    </row>
+    <row r="280" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D280" s="1">
+        <v>44144</v>
+      </c>
+    </row>
+    <row r="281" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D281" s="1">
+        <v>44145</v>
+      </c>
+    </row>
+    <row r="282" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D282" s="1">
+        <v>44146</v>
+      </c>
+    </row>
+    <row r="283" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D283" s="1">
+        <v>44147</v>
+      </c>
+    </row>
+    <row r="284" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D284" s="1">
+        <v>44148</v>
+      </c>
+    </row>
+    <row r="285" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D285" s="1">
+        <v>44151</v>
+      </c>
+    </row>
+    <row r="286" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D286" s="1">
+        <v>44152</v>
+      </c>
+    </row>
+    <row r="287" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D287" s="1">
+        <v>44153</v>
+      </c>
+    </row>
+    <row r="288" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D288" s="1">
+        <v>44154</v>
+      </c>
+    </row>
+    <row r="289" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D289" s="1">
+        <v>44155</v>
+      </c>
+    </row>
+    <row r="290" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D290" s="1">
+        <v>44158</v>
+      </c>
+    </row>
+    <row r="291" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D291" s="1">
+        <v>44159</v>
+      </c>
+    </row>
+    <row r="292" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D292" s="1">
+        <v>44160</v>
+      </c>
+    </row>
+    <row r="293" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D293" s="1">
+        <v>44161</v>
+      </c>
+    </row>
+    <row r="294" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="E294" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C12DF9A-38B2-4C14-8460-2F3CC36E3E92}">
-  <dimension ref="A1:A8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>460</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D168612-759E-4AAF-B82D-FF8921C18C50}">
-  <dimension ref="A1:A19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="A7" ca="1">IF(ISBLANK(INDIRECT("Cities!A"&amp;ROW(A7))),INDIRECT("Repeat!A"&amp;(ROWS($A$2:A7)-(COUNTA(Cities!A:A)-2))),Cities!A7)</f>
-        <v>F</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="A8" ca="1">IF(ISBLANK(INDIRECT("Cities!A"&amp;ROW(A8))),INDIRECT("Repeat!A"&amp;(ROWS($A$2:A8)-(COUNTA(Cities!A:A)-2))),Cities!A8)</f>
-        <v>G</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="A9" ca="1">IF(ISBLANK(INDIRECT("Cities!A"&amp;ROW(A9))),INDIRECT("Repeat!A"&amp;(ROWS($A$2:A9)-(COUNTA(Cities!A:A)-2))),Cities!A9)</f>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="A10" ca="1">IF(ISBLANK(INDIRECT("Cities!A"&amp;ROW(A10))),INDIRECT("Repeat!A"&amp;(ROWS($A$2:A10)-(COUNTA(Cities!A:A)-2))),Cities!A10)</f>
-        <v>B</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="A11" ca="1">IF(ISBLANK(INDIRECT("Cities!A"&amp;ROW(A11))),INDIRECT("Repeat!A"&amp;(ROWS($A$2:A11)-(COUNTA(Cities!A:A)-2))),Cities!A11)</f>
-        <v>C</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="A12" ca="1">IF(ISBLANK(INDIRECT("Cities!A"&amp;ROW(A12))),INDIRECT("Repeat!A"&amp;(ROWS($A$2:A12)-(COUNTA(Cities!A:A)-2))),Cities!A12)</f>
-        <v>D</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="A13" ca="1">IF(ISBLANK(INDIRECT("Cities!A"&amp;ROW(A13))),INDIRECT("Repeat!A"&amp;(ROWS($A$2:A13)-(COUNTA(Cities!A:A)-2))),Cities!A13)</f>
-        <v>E</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="A14" ca="1">IF(ISBLANK(INDIRECT("Cities!A"&amp;ROW(A14))),INDIRECT("Repeat!A"&amp;(ROWS($A$2:A14)-(COUNTA(Cities!A:A)-2))),Cities!A14)</f>
-        <v>F</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="A15" ca="1">IF(ISBLANK(INDIRECT("Cities!A"&amp;ROW(A15))),INDIRECT("Repeat!A"&amp;(ROWS($A$2:A15)-(COUNTA(Cities!A:A)-2))),Cities!A15)</f>
-        <v>G</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="A16" ca="1">IF(ISBLANK(INDIRECT("Cities!A"&amp;ROW(A16))),INDIRECT("Repeat!A"&amp;(ROWS($A$2:A16)-(COUNTA(Cities!A:A)-2))),Cities!A16)</f>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="A17" ca="1">IF(ISBLANK(INDIRECT("Cities!A"&amp;ROW(A17))),INDIRECT("Repeat!A"&amp;(ROWS($A$2:A17)-(COUNTA(Cities!A:A)-2))),Cities!A17)</f>
-        <v>B</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="A18" ca="1">IF(ISBLANK(INDIRECT("Cities!A"&amp;ROW(A18))),INDIRECT("Repeat!A"&amp;(ROWS($A$2:A18)-(COUNTA(Cities!A:A)-2))),Cities!A18)</f>
-        <v>C</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="str" cm="1">
-        <f t="array" aca="1" ref="A19" ca="1">IF(ISBLANK(INDIRECT("Cities!A"&amp;ROW(A19))),INDIRECT("Repeat!A"&amp;(ROWS($A$2:A19)-(COUNTA(Cities!A:A)-2))),Cities!A19)</f>
-        <v>D</v>
-      </c>
-    </row>
-  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>